<commit_message>
Optimize the available files
Improve the performance and efficiency of the available files
</commit_message>
<xml_diff>
--- a/1QnQ_Test/1Software_TESTING/PmP/Test Case/1PMP_TC_Project Detail.xlsx
+++ b/1QnQ_Test/1Software_TESTING/PmP/Test Case/1PMP_TC_Project Detail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1QnQ_Test\1Software_TESTING\PmP\Test Case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test Files\Test-Files\1QnQ_Test\1Software_TESTING\PmP\Test Case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663B09E5-BAA1-4336-9F90-3B5F4345A5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC595F3-32F8-40D5-BA50-06F6341B41BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="1" r:id="rId1"/>
@@ -2153,18 +2153,18 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="41.42578125" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="41.44140625" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="7:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="7:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="7:11" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="7:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="7:11" ht="46.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G9" s="35" t="s">
         <v>412</v>
       </c>
@@ -2173,18 +2173,18 @@
       <c r="J9" s="36"/>
       <c r="K9" s="37"/>
     </row>
-    <row r="10" spans="7:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="7:11" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="7:11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="7:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="G13" s="38"/>
       <c r="H13" s="38"/>
       <c r="I13" s="38"/>
       <c r="J13" s="38"/>
       <c r="K13" s="38"/>
     </row>
-    <row r="14" spans="7:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="7:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="7:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="7:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G15" s="39" t="s">
         <v>0</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="7:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="7:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G16" s="40"/>
       <c r="H16" s="40"/>
       <c r="I16" s="21" t="s">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="K16" s="43"/>
     </row>
-    <row r="17" spans="7:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G17" s="2">
         <v>1</v>
       </c>
@@ -2227,10 +2227,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:11" x14ac:dyDescent="0.3">
       <c r="J18" s="5"/>
     </row>
-    <row r="24" spans="7:11" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="7:11" hidden="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="G9:K9"/>
@@ -2249,28 +2249,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{859CFD0A-2144-4C68-8D17-11D0822EF067}">
   <dimension ref="A1:CO491"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D481" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I490" sqref="I490"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="12"/>
-    <col min="2" max="2" width="8.7109375" style="12" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="1.7109375" style="12" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="12"/>
+    <col min="2" max="2" width="8.6640625" style="12" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="1.6640625" style="12" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="12" customWidth="1"/>
     <col min="5" max="5" width="53" style="9" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" style="12" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="79.28515625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="59.7109375" style="9" customWidth="1"/>
-    <col min="11" max="12" width="17.85546875" style="12" customWidth="1"/>
-    <col min="13" max="13" width="24.28515625" style="12" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="12"/>
+    <col min="6" max="6" width="4.88671875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" style="12" customWidth="1"/>
+    <col min="9" max="9" width="79.33203125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="59.6640625" style="9" customWidth="1"/>
+    <col min="11" max="12" width="17.88671875" style="12" customWidth="1"/>
+    <col min="13" max="13" width="24.33203125" style="12" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:93" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:93" s="8" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:93" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:93" s="9" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <f>SUBTOTAL(3,$E$2:E2)</f>
         <v>1</v>
@@ -2394,7 +2394,7 @@
       <c r="CN2" s="13"/>
       <c r="CO2" s="13"/>
     </row>
-    <row r="3" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H3" s="12" t="s">
         <v>22</v>
       </c>
@@ -2488,7 +2488,7 @@
       <c r="CN3" s="13"/>
       <c r="CO3" s="13"/>
     </row>
-    <row r="4" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H4" s="12" t="s">
         <v>23</v>
       </c>
@@ -2582,7 +2582,7 @@
       <c r="CN4" s="13"/>
       <c r="CO4" s="13"/>
     </row>
-    <row r="5" spans="1:93" s="9" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:93" s="9" customFormat="1" ht="69" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <f>SUBTOTAL(3,$E$2:E5)</f>
         <v>2</v>
@@ -2667,7 +2667,7 @@
       <c r="CN5" s="13"/>
       <c r="CO5" s="13"/>
     </row>
-    <row r="6" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H6" s="12" t="s">
         <v>22</v>
       </c>
@@ -2761,7 +2761,7 @@
       <c r="CN6" s="13"/>
       <c r="CO6" s="13"/>
     </row>
-    <row r="7" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H7" s="12" t="s">
         <v>23</v>
       </c>
@@ -2855,7 +2855,7 @@
       <c r="CN7" s="13"/>
       <c r="CO7" s="13"/>
     </row>
-    <row r="8" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H8" s="12" t="s">
         <v>25</v>
       </c>
@@ -2949,7 +2949,7 @@
       <c r="CN8" s="13"/>
       <c r="CO8" s="13"/>
     </row>
-    <row r="9" spans="1:93" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:93" s="9" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <f>SUBTOTAL(3,$E$2:E9)</f>
         <v>3</v>
@@ -3034,7 +3034,7 @@
       <c r="CN9" s="13"/>
       <c r="CO9" s="13"/>
     </row>
-    <row r="10" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H10" s="12" t="s">
         <v>22</v>
       </c>
@@ -3128,7 +3128,7 @@
       <c r="CN10" s="13"/>
       <c r="CO10" s="13"/>
     </row>
-    <row r="11" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H11" s="12" t="s">
         <v>23</v>
       </c>
@@ -3222,7 +3222,7 @@
       <c r="CN11" s="13"/>
       <c r="CO11" s="13"/>
     </row>
-    <row r="12" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H12" s="12" t="s">
         <v>25</v>
       </c>
@@ -3316,7 +3316,7 @@
       <c r="CN12" s="13"/>
       <c r="CO12" s="13"/>
     </row>
-    <row r="13" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H13" s="12" t="s">
         <v>28</v>
       </c>
@@ -3410,7 +3410,7 @@
       <c r="CN13" s="13"/>
       <c r="CO13" s="13"/>
     </row>
-    <row r="14" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H14" s="12" t="s">
         <v>30</v>
       </c>
@@ -3504,7 +3504,7 @@
       <c r="CN14" s="13"/>
       <c r="CO14" s="13"/>
     </row>
-    <row r="15" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H15" s="12" t="s">
         <v>32</v>
       </c>
@@ -3598,7 +3598,7 @@
       <c r="CN15" s="13"/>
       <c r="CO15" s="13"/>
     </row>
-    <row r="16" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <f>SUBTOTAL(3,$E$2:E16)</f>
         <v>4</v>
@@ -3709,7 +3709,7 @@
       <c r="CN16" s="13"/>
       <c r="CO16" s="13"/>
     </row>
-    <row r="17" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H17" s="12" t="s">
         <v>22</v>
       </c>
@@ -3803,7 +3803,7 @@
       <c r="CN17" s="13"/>
       <c r="CO17" s="13"/>
     </row>
-    <row r="18" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3897,7 +3897,7 @@
       <c r="CN18" s="13"/>
       <c r="CO18" s="13"/>
     </row>
-    <row r="19" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H19" s="12" t="s">
         <v>25</v>
       </c>
@@ -3991,7 +3991,7 @@
       <c r="CN19" s="13"/>
       <c r="CO19" s="13"/>
     </row>
-    <row r="20" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <f>SUBTOTAL(3,$E$2:E20)</f>
         <v>5</v>
@@ -4102,7 +4102,7 @@
       <c r="CN20" s="13"/>
       <c r="CO20" s="13"/>
     </row>
-    <row r="21" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H21" s="12" t="s">
         <v>22</v>
       </c>
@@ -4196,7 +4196,7 @@
       <c r="CN21" s="13"/>
       <c r="CO21" s="13"/>
     </row>
-    <row r="22" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H22" s="12" t="s">
         <v>23</v>
       </c>
@@ -4290,7 +4290,7 @@
       <c r="CN22" s="13"/>
       <c r="CO22" s="13"/>
     </row>
-    <row r="23" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H23" s="12" t="s">
         <v>25</v>
       </c>
@@ -4384,7 +4384,7 @@
       <c r="CN23" s="13"/>
       <c r="CO23" s="13"/>
     </row>
-    <row r="24" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H24" s="12" t="s">
         <v>28</v>
       </c>
@@ -4478,7 +4478,7 @@
       <c r="CN24" s="13"/>
       <c r="CO24" s="13"/>
     </row>
-    <row r="25" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H25" s="12" t="s">
         <v>30</v>
       </c>
@@ -4572,7 +4572,7 @@
       <c r="CN25" s="13"/>
       <c r="CO25" s="13"/>
     </row>
-    <row r="26" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <f>SUBTOTAL(3,$E$2:E26)</f>
         <v>6</v>
@@ -4683,7 +4683,7 @@
       <c r="CN26" s="13"/>
       <c r="CO26" s="13"/>
     </row>
-    <row r="27" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H27" s="12" t="s">
         <v>22</v>
       </c>
@@ -4777,7 +4777,7 @@
       <c r="CN27" s="13"/>
       <c r="CO27" s="13"/>
     </row>
-    <row r="28" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H28" s="12" t="s">
         <v>23</v>
       </c>
@@ -4871,7 +4871,7 @@
       <c r="CN28" s="13"/>
       <c r="CO28" s="13"/>
     </row>
-    <row r="29" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H29" s="12" t="s">
         <v>25</v>
       </c>
@@ -4965,7 +4965,7 @@
       <c r="CN29" s="13"/>
       <c r="CO29" s="13"/>
     </row>
-    <row r="30" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H30" s="12" t="s">
         <v>28</v>
       </c>
@@ -5059,7 +5059,7 @@
       <c r="CN30" s="13"/>
       <c r="CO30" s="13"/>
     </row>
-    <row r="31" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <f>SUBTOTAL(3,$E$2:E31)</f>
         <v>7</v>
@@ -5170,7 +5170,7 @@
       <c r="CN31" s="13"/>
       <c r="CO31" s="13"/>
     </row>
-    <row r="32" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H32" s="12" t="s">
         <v>22</v>
       </c>
@@ -5264,7 +5264,7 @@
       <c r="CN32" s="13"/>
       <c r="CO32" s="13"/>
     </row>
-    <row r="33" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H33" s="12" t="s">
         <v>23</v>
       </c>
@@ -5358,7 +5358,7 @@
       <c r="CN33" s="13"/>
       <c r="CO33" s="13"/>
     </row>
-    <row r="34" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H34" s="12" t="s">
         <v>25</v>
       </c>
@@ -5452,7 +5452,7 @@
       <c r="CN34" s="13"/>
       <c r="CO34" s="13"/>
     </row>
-    <row r="35" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H35" s="12" t="s">
         <v>28</v>
       </c>
@@ -5546,7 +5546,7 @@
       <c r="CN35" s="13"/>
       <c r="CO35" s="13"/>
     </row>
-    <row r="36" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <f>SUBTOTAL(3,$E$2:E36)</f>
         <v>8</v>
@@ -5657,7 +5657,7 @@
       <c r="CN36" s="13"/>
       <c r="CO36" s="13"/>
     </row>
-    <row r="37" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H37" s="12" t="s">
         <v>22</v>
       </c>
@@ -5751,7 +5751,7 @@
       <c r="CN37" s="13"/>
       <c r="CO37" s="13"/>
     </row>
-    <row r="38" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H38" s="12" t="s">
         <v>23</v>
       </c>
@@ -5845,7 +5845,7 @@
       <c r="CN38" s="13"/>
       <c r="CO38" s="13"/>
     </row>
-    <row r="39" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H39" s="12" t="s">
         <v>25</v>
       </c>
@@ -5939,7 +5939,7 @@
       <c r="CN39" s="13"/>
       <c r="CO39" s="13"/>
     </row>
-    <row r="40" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H40" s="12" t="s">
         <v>28</v>
       </c>
@@ -6033,7 +6033,7 @@
       <c r="CN40" s="13"/>
       <c r="CO40" s="13"/>
     </row>
-    <row r="41" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <f>SUBTOTAL(3,$E$2:E41)</f>
         <v>9</v>
@@ -6144,7 +6144,7 @@
       <c r="CN41" s="13"/>
       <c r="CO41" s="13"/>
     </row>
-    <row r="42" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H42" s="12" t="s">
         <v>22</v>
       </c>
@@ -6238,7 +6238,7 @@
       <c r="CN42" s="13"/>
       <c r="CO42" s="13"/>
     </row>
-    <row r="43" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H43" s="12" t="s">
         <v>23</v>
       </c>
@@ -6332,7 +6332,7 @@
       <c r="CN43" s="13"/>
       <c r="CO43" s="13"/>
     </row>
-    <row r="44" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H44" s="12" t="s">
         <v>25</v>
       </c>
@@ -6426,7 +6426,7 @@
       <c r="CN44" s="13"/>
       <c r="CO44" s="13"/>
     </row>
-    <row r="45" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H45" s="12" t="s">
         <v>28</v>
       </c>
@@ -6520,7 +6520,7 @@
       <c r="CN45" s="13"/>
       <c r="CO45" s="13"/>
     </row>
-    <row r="46" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H46" s="12" t="s">
         <v>30</v>
       </c>
@@ -6614,7 +6614,7 @@
       <c r="CN46" s="13"/>
       <c r="CO46" s="13"/>
     </row>
-    <row r="47" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H47" s="12" t="s">
         <v>32</v>
       </c>
@@ -6708,7 +6708,7 @@
       <c r="CN47" s="13"/>
       <c r="CO47" s="13"/>
     </row>
-    <row r="48" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H48" s="12" t="s">
         <v>72</v>
       </c>
@@ -6802,7 +6802,7 @@
       <c r="CN48" s="13"/>
       <c r="CO48" s="13"/>
     </row>
-    <row r="49" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <f>SUBTOTAL(3,$E$2:E49)</f>
         <v>10</v>
@@ -6912,7 +6912,7 @@
       <c r="CN49" s="13"/>
       <c r="CO49" s="13"/>
     </row>
-    <row r="50" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H50" s="12" t="s">
         <v>22</v>
       </c>
@@ -7006,7 +7006,7 @@
       <c r="CN50" s="13"/>
       <c r="CO50" s="13"/>
     </row>
-    <row r="51" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H51" s="12" t="s">
         <v>23</v>
       </c>
@@ -7100,7 +7100,7 @@
       <c r="CN51" s="13"/>
       <c r="CO51" s="13"/>
     </row>
-    <row r="52" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H52" s="12" t="s">
         <v>25</v>
       </c>
@@ -7194,7 +7194,7 @@
       <c r="CN52" s="13"/>
       <c r="CO52" s="13"/>
     </row>
-    <row r="53" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H53" s="12" t="s">
         <v>28</v>
       </c>
@@ -7288,7 +7288,7 @@
       <c r="CN53" s="13"/>
       <c r="CO53" s="13"/>
     </row>
-    <row r="54" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H54" s="12" t="s">
         <v>30</v>
       </c>
@@ -7382,7 +7382,7 @@
       <c r="CN54" s="13"/>
       <c r="CO54" s="13"/>
     </row>
-    <row r="55" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H55" s="12" t="s">
         <v>32</v>
       </c>
@@ -7476,7 +7476,7 @@
       <c r="CN55" s="13"/>
       <c r="CO55" s="13"/>
     </row>
-    <row r="56" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <f>SUBTOTAL(3,$E$2:E56)</f>
         <v>11</v>
@@ -7587,7 +7587,7 @@
       <c r="CN56" s="13"/>
       <c r="CO56" s="13"/>
     </row>
-    <row r="57" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H57" s="12" t="s">
         <v>22</v>
       </c>
@@ -7681,7 +7681,7 @@
       <c r="CN57" s="13"/>
       <c r="CO57" s="13"/>
     </row>
-    <row r="58" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H58" s="12" t="s">
         <v>23</v>
       </c>
@@ -7775,7 +7775,7 @@
       <c r="CN58" s="13"/>
       <c r="CO58" s="13"/>
     </row>
-    <row r="59" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H59" s="12" t="s">
         <v>25</v>
       </c>
@@ -7869,7 +7869,7 @@
       <c r="CN59" s="13"/>
       <c r="CO59" s="13"/>
     </row>
-    <row r="60" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H60" s="12" t="s">
         <v>28</v>
       </c>
@@ -7963,7 +7963,7 @@
       <c r="CN60" s="13"/>
       <c r="CO60" s="13"/>
     </row>
-    <row r="61" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
         <f>SUBTOTAL(3,$E$2:E61)</f>
         <v>12</v>
@@ -8074,7 +8074,7 @@
       <c r="CN61" s="13"/>
       <c r="CO61" s="13"/>
     </row>
-    <row r="62" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H62" s="12" t="s">
         <v>22</v>
       </c>
@@ -8168,7 +8168,7 @@
       <c r="CN62" s="13"/>
       <c r="CO62" s="13"/>
     </row>
-    <row r="63" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H63" s="12" t="s">
         <v>23</v>
       </c>
@@ -8262,7 +8262,7 @@
       <c r="CN63" s="13"/>
       <c r="CO63" s="13"/>
     </row>
-    <row r="64" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H64" s="12" t="s">
         <v>25</v>
       </c>
@@ -8356,7 +8356,7 @@
       <c r="CN64" s="13"/>
       <c r="CO64" s="13"/>
     </row>
-    <row r="65" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H65" s="12" t="s">
         <v>28</v>
       </c>
@@ -8450,7 +8450,7 @@
       <c r="CN65" s="13"/>
       <c r="CO65" s="13"/>
     </row>
-    <row r="66" spans="1:93" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:93" s="9" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <f>SUBTOTAL(3,$E$2:E66)</f>
         <v>13</v>
@@ -8534,7 +8534,7 @@
       <c r="CN66" s="13"/>
       <c r="CO66" s="13"/>
     </row>
-    <row r="67" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="12"/>
       <c r="E67" s="9" t="s">
         <v>5</v>
@@ -8607,7 +8607,7 @@
       <c r="CN67" s="13"/>
       <c r="CO67" s="13"/>
     </row>
-    <row r="68" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="12"/>
       <c r="F68" s="12"/>
       <c r="G68" s="12"/>
@@ -8677,7 +8677,7 @@
       <c r="CN68" s="13"/>
       <c r="CO68" s="13"/>
     </row>
-    <row r="69" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="12"/>
       <c r="F69" s="12"/>
       <c r="G69" s="12"/>
@@ -8747,7 +8747,7 @@
       <c r="CN69" s="13"/>
       <c r="CO69" s="13"/>
     </row>
-    <row r="70" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="12"/>
       <c r="F70" s="12"/>
       <c r="G70" s="12"/>
@@ -8817,7 +8817,7 @@
       <c r="CN70" s="13"/>
       <c r="CO70" s="13"/>
     </row>
-    <row r="71" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <f>SUBTOTAL(3,$E$2:E71)</f>
         <v>15</v>
@@ -8929,7 +8929,7 @@
       <c r="CN71" s="13"/>
       <c r="CO71" s="13"/>
     </row>
-    <row r="72" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H72" s="9" t="s">
         <v>22</v>
       </c>
@@ -9023,7 +9023,7 @@
       <c r="CN72" s="13"/>
       <c r="CO72" s="13"/>
     </row>
-    <row r="73" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H73" s="9" t="s">
         <v>23</v>
       </c>
@@ -9117,7 +9117,7 @@
       <c r="CN73" s="13"/>
       <c r="CO73" s="13"/>
     </row>
-    <row r="74" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H74" s="9" t="s">
         <v>25</v>
       </c>
@@ -9211,7 +9211,7 @@
       <c r="CN74" s="13"/>
       <c r="CO74" s="13"/>
     </row>
-    <row r="75" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H75" s="9" t="s">
         <v>28</v>
       </c>
@@ -9305,7 +9305,7 @@
       <c r="CN75" s="13"/>
       <c r="CO75" s="13"/>
     </row>
-    <row r="76" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H76" s="9" t="s">
         <v>30</v>
       </c>
@@ -9399,7 +9399,7 @@
       <c r="CN76" s="13"/>
       <c r="CO76" s="13"/>
     </row>
-    <row r="77" spans="1:93" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:93" s="9" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <f>SUBTOTAL(3,$E$2:E77)</f>
         <v>16</v>
@@ -9483,7 +9483,7 @@
       <c r="CN77" s="13"/>
       <c r="CO77" s="13"/>
     </row>
-    <row r="78" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="12"/>
       <c r="F78" s="12"/>
       <c r="G78" s="12"/>
@@ -9553,7 +9553,7 @@
       <c r="CN78" s="13"/>
       <c r="CO78" s="13"/>
     </row>
-    <row r="79" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="12"/>
       <c r="F79" s="12"/>
       <c r="G79" s="12"/>
@@ -9623,7 +9623,7 @@
       <c r="CN79" s="13"/>
       <c r="CO79" s="13"/>
     </row>
-    <row r="80" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="12"/>
       <c r="F80" s="12"/>
       <c r="G80" s="12"/>
@@ -9693,7 +9693,7 @@
       <c r="CN80" s="13"/>
       <c r="CO80" s="13"/>
     </row>
-    <row r="81" spans="1:93" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:93" s="9" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B81" s="12"/>
       <c r="F81" s="12"/>
       <c r="G81" s="12"/>
@@ -9763,7 +9763,7 @@
       <c r="CN81" s="13"/>
       <c r="CO81" s="13"/>
     </row>
-    <row r="82" spans="1:93" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:93" s="9" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <f>SUBTOTAL(3,$E$2:E82)</f>
         <v>17</v>
@@ -9847,7 +9847,7 @@
       <c r="CN82" s="13"/>
       <c r="CO82" s="13"/>
     </row>
-    <row r="83" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="12"/>
       <c r="F83" s="12"/>
       <c r="G83" s="12"/>
@@ -9917,7 +9917,7 @@
       <c r="CN83" s="13"/>
       <c r="CO83" s="13"/>
     </row>
-    <row r="84" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="12"/>
       <c r="F84" s="12"/>
       <c r="G84" s="12"/>
@@ -9987,7 +9987,7 @@
       <c r="CN84" s="13"/>
       <c r="CO84" s="13"/>
     </row>
-    <row r="85" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="12"/>
       <c r="F85" s="12"/>
       <c r="G85" s="12"/>
@@ -10057,7 +10057,7 @@
       <c r="CN85" s="13"/>
       <c r="CO85" s="13"/>
     </row>
-    <row r="86" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B86" s="12"/>
       <c r="F86" s="12"/>
       <c r="G86" s="12"/>
@@ -10127,7 +10127,7 @@
       <c r="CN86" s="13"/>
       <c r="CO86" s="13"/>
     </row>
-    <row r="87" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="23"/>
       <c r="B87" s="24"/>
       <c r="C87" s="23"/>
@@ -10201,7 +10201,7 @@
       <c r="CN87" s="13"/>
       <c r="CO87" s="13"/>
     </row>
-    <row r="88" spans="1:93" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:93" s="9" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <f>SUBTOTAL(3,$E$2:E88)</f>
         <v>18</v>
@@ -10285,7 +10285,7 @@
       <c r="CN88" s="13"/>
       <c r="CO88" s="13"/>
     </row>
-    <row r="89" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="12"/>
       <c r="E89" s="9" t="s">
         <v>5</v>
@@ -10358,7 +10358,7 @@
       <c r="CN89" s="13"/>
       <c r="CO89" s="13"/>
     </row>
-    <row r="90" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="12"/>
       <c r="F90" s="12"/>
       <c r="G90" s="12"/>
@@ -10428,7 +10428,7 @@
       <c r="CN90" s="13"/>
       <c r="CO90" s="13"/>
     </row>
-    <row r="91" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="12"/>
       <c r="F91" s="12"/>
       <c r="G91" s="12"/>
@@ -10498,7 +10498,7 @@
       <c r="CN91" s="13"/>
       <c r="CO91" s="13"/>
     </row>
-    <row r="92" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="12"/>
       <c r="F92" s="12"/>
       <c r="G92" s="12"/>
@@ -10568,7 +10568,7 @@
       <c r="CN92" s="13"/>
       <c r="CO92" s="13"/>
     </row>
-    <row r="93" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
         <f>SUBTOTAL(3,$E$2:E93)</f>
         <v>20</v>
@@ -10680,7 +10680,7 @@
       <c r="CN93" s="13"/>
       <c r="CO93" s="13"/>
     </row>
-    <row r="94" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H94" s="9" t="s">
         <v>22</v>
       </c>
@@ -10774,7 +10774,7 @@
       <c r="CN94" s="13"/>
       <c r="CO94" s="13"/>
     </row>
-    <row r="95" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H95" s="9" t="s">
         <v>23</v>
       </c>
@@ -10868,7 +10868,7 @@
       <c r="CN95" s="13"/>
       <c r="CO95" s="13"/>
     </row>
-    <row r="96" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H96" s="9" t="s">
         <v>25</v>
       </c>
@@ -10962,7 +10962,7 @@
       <c r="CN96" s="13"/>
       <c r="CO96" s="13"/>
     </row>
-    <row r="97" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H97" s="9" t="s">
         <v>28</v>
       </c>
@@ -11056,7 +11056,7 @@
       <c r="CN97" s="13"/>
       <c r="CO97" s="13"/>
     </row>
-    <row r="98" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H98" s="9" t="s">
         <v>30</v>
       </c>
@@ -11150,7 +11150,7 @@
       <c r="CN98" s="13"/>
       <c r="CO98" s="13"/>
     </row>
-    <row r="99" spans="1:93" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:93" s="9" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A99" s="9">
         <f>SUBTOTAL(3,$E$2:E99)</f>
         <v>21</v>
@@ -11234,7 +11234,7 @@
       <c r="CN99" s="13"/>
       <c r="CO99" s="13"/>
     </row>
-    <row r="100" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="12"/>
       <c r="F100" s="12"/>
       <c r="G100" s="12"/>
@@ -11304,7 +11304,7 @@
       <c r="CN100" s="13"/>
       <c r="CO100" s="13"/>
     </row>
-    <row r="101" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="12"/>
       <c r="F101" s="12"/>
       <c r="G101" s="12"/>
@@ -11374,7 +11374,7 @@
       <c r="CN101" s="13"/>
       <c r="CO101" s="13"/>
     </row>
-    <row r="102" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B102" s="12"/>
       <c r="F102" s="12"/>
       <c r="G102" s="12"/>
@@ -11444,7 +11444,7 @@
       <c r="CN102" s="13"/>
       <c r="CO102" s="13"/>
     </row>
-    <row r="103" spans="1:93" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:93" s="9" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B103" s="12"/>
       <c r="F103" s="12"/>
       <c r="G103" s="12"/>
@@ -11514,7 +11514,7 @@
       <c r="CN103" s="13"/>
       <c r="CO103" s="13"/>
     </row>
-    <row r="104" spans="1:93" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:93" s="9" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A104" s="9">
         <f>SUBTOTAL(3,$E$2:E104)</f>
         <v>22</v>
@@ -11598,7 +11598,7 @@
       <c r="CN104" s="13"/>
       <c r="CO104" s="13"/>
     </row>
-    <row r="105" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B105" s="12"/>
       <c r="F105" s="12"/>
       <c r="G105" s="12"/>
@@ -11668,7 +11668,7 @@
       <c r="CN105" s="13"/>
       <c r="CO105" s="13"/>
     </row>
-    <row r="106" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B106" s="12"/>
       <c r="F106" s="12"/>
       <c r="G106" s="12"/>
@@ -11738,7 +11738,7 @@
       <c r="CN106" s="13"/>
       <c r="CO106" s="13"/>
     </row>
-    <row r="107" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B107" s="12"/>
       <c r="F107" s="12"/>
       <c r="G107" s="12"/>
@@ -11808,7 +11808,7 @@
       <c r="CN107" s="13"/>
       <c r="CO107" s="13"/>
     </row>
-    <row r="108" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B108" s="12"/>
       <c r="F108" s="12"/>
       <c r="G108" s="12"/>
@@ -11878,7 +11878,7 @@
       <c r="CN108" s="13"/>
       <c r="CO108" s="13"/>
     </row>
-    <row r="109" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="23"/>
       <c r="B109" s="24"/>
       <c r="C109" s="23"/>
@@ -11952,7 +11952,7 @@
       <c r="CN109" s="13"/>
       <c r="CO109" s="13"/>
     </row>
-    <row r="110" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A110" s="9">
         <f>SUBTOTAL(3,$E$2:E110)</f>
         <v>23</v>
@@ -12064,7 +12064,7 @@
       <c r="CN110" s="13"/>
       <c r="CO110" s="13"/>
     </row>
-    <row r="111" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H111" s="9" t="s">
         <v>22</v>
       </c>
@@ -12158,7 +12158,7 @@
       <c r="CN111" s="13"/>
       <c r="CO111" s="13"/>
     </row>
-    <row r="112" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H112" s="9" t="s">
         <v>23</v>
       </c>
@@ -12252,7 +12252,7 @@
       <c r="CN112" s="13"/>
       <c r="CO112" s="13"/>
     </row>
-    <row r="113" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H113" s="9" t="s">
         <v>25</v>
       </c>
@@ -12346,7 +12346,7 @@
       <c r="CN113" s="13"/>
       <c r="CO113" s="13"/>
     </row>
-    <row r="114" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H114" s="9" t="s">
         <v>28</v>
       </c>
@@ -12440,7 +12440,7 @@
       <c r="CN114" s="13"/>
       <c r="CO114" s="13"/>
     </row>
-    <row r="115" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H115" s="9" t="s">
         <v>30</v>
       </c>
@@ -12534,7 +12534,7 @@
       <c r="CN115" s="13"/>
       <c r="CO115" s="13"/>
     </row>
-    <row r="116" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A116" s="9">
         <f>SUBTOTAL(3,$E$2:E116)</f>
         <v>24</v>
@@ -12646,7 +12646,7 @@
       <c r="CN116" s="13"/>
       <c r="CO116" s="13"/>
     </row>
-    <row r="117" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H117" s="9" t="s">
         <v>22</v>
       </c>
@@ -12740,7 +12740,7 @@
       <c r="CN117" s="13"/>
       <c r="CO117" s="13"/>
     </row>
-    <row r="118" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H118" s="9" t="s">
         <v>23</v>
       </c>
@@ -12834,7 +12834,7 @@
       <c r="CN118" s="13"/>
       <c r="CO118" s="13"/>
     </row>
-    <row r="119" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H119" s="9" t="s">
         <v>25</v>
       </c>
@@ -12928,7 +12928,7 @@
       <c r="CN119" s="13"/>
       <c r="CO119" s="13"/>
     </row>
-    <row r="120" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H120" s="9" t="s">
         <v>28</v>
       </c>
@@ -13022,7 +13022,7 @@
       <c r="CN120" s="13"/>
       <c r="CO120" s="13"/>
     </row>
-    <row r="121" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H121" s="9" t="s">
         <v>30</v>
       </c>
@@ -13116,7 +13116,7 @@
       <c r="CN121" s="13"/>
       <c r="CO121" s="13"/>
     </row>
-    <row r="122" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H122" s="9" t="s">
         <v>32</v>
       </c>
@@ -13210,7 +13210,7 @@
       <c r="CN122" s="13"/>
       <c r="CO122" s="13"/>
     </row>
-    <row r="123" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H123" s="9" t="s">
         <v>72</v>
       </c>
@@ -13304,7 +13304,7 @@
       <c r="CN123" s="13"/>
       <c r="CO123" s="13"/>
     </row>
-    <row r="124" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H124" s="9" t="s">
         <v>75</v>
       </c>
@@ -13398,7 +13398,7 @@
       <c r="CN124" s="13"/>
       <c r="CO124" s="13"/>
     </row>
-    <row r="125" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H125" s="9" t="s">
         <v>103</v>
       </c>
@@ -13492,7 +13492,7 @@
       <c r="CN125" s="13"/>
       <c r="CO125" s="13"/>
     </row>
-    <row r="126" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H126" s="9" t="s">
         <v>104</v>
       </c>
@@ -13586,7 +13586,7 @@
       <c r="CN126" s="13"/>
       <c r="CO126" s="13"/>
     </row>
-    <row r="127" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A127" s="9">
         <f>SUBTOTAL(3,$E$2:E127)</f>
         <v>25</v>
@@ -13698,7 +13698,7 @@
       <c r="CN127" s="13"/>
       <c r="CO127" s="13"/>
     </row>
-    <row r="128" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H128" s="9" t="s">
         <v>22</v>
       </c>
@@ -13792,7 +13792,7 @@
       <c r="CN128" s="13"/>
       <c r="CO128" s="13"/>
     </row>
-    <row r="129" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H129" s="9" t="s">
         <v>23</v>
       </c>
@@ -13886,7 +13886,7 @@
       <c r="CN129" s="13"/>
       <c r="CO129" s="13"/>
     </row>
-    <row r="130" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H130" s="9" t="s">
         <v>25</v>
       </c>
@@ -13980,7 +13980,7 @@
       <c r="CN130" s="13"/>
       <c r="CO130" s="13"/>
     </row>
-    <row r="131" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H131" s="9" t="s">
         <v>28</v>
       </c>
@@ -14074,7 +14074,7 @@
       <c r="CN131" s="13"/>
       <c r="CO131" s="13"/>
     </row>
-    <row r="132" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H132" s="9" t="s">
         <v>30</v>
       </c>
@@ -14168,7 +14168,7 @@
       <c r="CN132" s="13"/>
       <c r="CO132" s="13"/>
     </row>
-    <row r="133" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H133" s="9" t="s">
         <v>32</v>
       </c>
@@ -14262,7 +14262,7 @@
       <c r="CN133" s="13"/>
       <c r="CO133" s="13"/>
     </row>
-    <row r="134" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H134" s="9" t="s">
         <v>72</v>
       </c>
@@ -14356,7 +14356,7 @@
       <c r="CN134" s="13"/>
       <c r="CO134" s="13"/>
     </row>
-    <row r="135" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H135" s="9" t="s">
         <v>75</v>
       </c>
@@ -14450,7 +14450,7 @@
       <c r="CN135" s="13"/>
       <c r="CO135" s="13"/>
     </row>
-    <row r="136" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H136" s="9" t="s">
         <v>103</v>
       </c>
@@ -14544,7 +14544,7 @@
       <c r="CN136" s="13"/>
       <c r="CO136" s="13"/>
     </row>
-    <row r="137" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H137" s="9" t="s">
         <v>104</v>
       </c>
@@ -14638,7 +14638,7 @@
       <c r="CN137" s="13"/>
       <c r="CO137" s="13"/>
     </row>
-    <row r="138" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:93" x14ac:dyDescent="0.25">
       <c r="E138" s="12"/>
       <c r="H138" s="9" t="s">
         <v>105</v>
@@ -14733,7 +14733,7 @@
       <c r="CN138" s="13"/>
       <c r="CO138" s="13"/>
     </row>
-    <row r="139" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A139" s="9">
         <f>SUBTOTAL(3,$E$2:E139)</f>
         <v>26</v>
@@ -14845,7 +14845,7 @@
       <c r="CN139" s="13"/>
       <c r="CO139" s="13"/>
     </row>
-    <row r="140" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H140" s="9" t="s">
         <v>22</v>
       </c>
@@ -14939,7 +14939,7 @@
       <c r="CN140" s="13"/>
       <c r="CO140" s="13"/>
     </row>
-    <row r="141" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H141" s="9" t="s">
         <v>23</v>
       </c>
@@ -15033,7 +15033,7 @@
       <c r="CN141" s="13"/>
       <c r="CO141" s="13"/>
     </row>
-    <row r="142" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H142" s="9" t="s">
         <v>25</v>
       </c>
@@ -15127,7 +15127,7 @@
       <c r="CN142" s="13"/>
       <c r="CO142" s="13"/>
     </row>
-    <row r="143" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H143" s="9" t="s">
         <v>28</v>
       </c>
@@ -15221,7 +15221,7 @@
       <c r="CN143" s="13"/>
       <c r="CO143" s="13"/>
     </row>
-    <row r="144" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A144" s="24"/>
       <c r="B144" s="24"/>
       <c r="C144" s="24"/>
@@ -15322,7 +15322,7 @@
       <c r="CN144" s="13"/>
       <c r="CO144" s="13"/>
     </row>
-    <row r="145" spans="1:10" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A145" s="9">
         <f>SUBTOTAL(3,$E$2:E145)</f>
         <v>27</v>
@@ -15351,7 +15351,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H146" s="9" t="s">
         <v>22</v>
       </c>
@@ -15362,7 +15362,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H147" s="9" t="s">
         <v>23</v>
       </c>
@@ -15373,7 +15373,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H148" s="9" t="s">
         <v>25</v>
       </c>
@@ -15384,7 +15384,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="156.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:10" ht="151.80000000000001" x14ac:dyDescent="0.25">
       <c r="H149" s="9" t="s">
         <v>28</v>
       </c>
@@ -15395,7 +15395,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="156.75" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:10" ht="151.80000000000001" x14ac:dyDescent="0.25">
       <c r="H150" s="9" t="s">
         <v>30</v>
       </c>
@@ -15406,7 +15406,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A151" s="9">
         <f>SUBTOTAL(3,$E$2:E151)</f>
         <v>28</v>
@@ -15435,7 +15435,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H152" s="9" t="s">
         <v>22</v>
       </c>
@@ -15446,7 +15446,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H153" s="9" t="s">
         <v>23</v>
       </c>
@@ -15457,7 +15457,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H154" s="9" t="s">
         <v>25</v>
       </c>
@@ -15468,7 +15468,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="155" spans="1:10" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H155" s="12" t="s">
         <v>28</v>
       </c>
@@ -15479,7 +15479,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="156" spans="1:10" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A156" s="9">
         <f>SUBTOTAL(3,$E$2:E156)</f>
         <v>29</v>
@@ -15508,7 +15508,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H157" s="9" t="s">
         <v>22</v>
       </c>
@@ -15519,7 +15519,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H158" s="9" t="s">
         <v>23</v>
       </c>
@@ -15530,7 +15530,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H159" s="9" t="s">
         <v>25</v>
       </c>
@@ -15541,7 +15541,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H160" s="9" t="s">
         <v>28</v>
       </c>
@@ -15552,7 +15552,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="161" spans="1:10" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H161" s="9" t="s">
         <v>30</v>
       </c>
@@ -15563,7 +15563,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H162" s="9" t="s">
         <v>32</v>
       </c>
@@ -15574,7 +15574,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A163" s="9">
         <f>SUBTOTAL(3,$E$2:E163)</f>
         <v>30</v>
@@ -15603,7 +15603,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H164" s="9" t="s">
         <v>22</v>
       </c>
@@ -15614,7 +15614,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H165" s="9" t="s">
         <v>23</v>
       </c>
@@ -15625,7 +15625,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H166" s="9" t="s">
         <v>25</v>
       </c>
@@ -15636,7 +15636,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="167" spans="1:10" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H167" s="9" t="s">
         <v>28</v>
       </c>
@@ -15647,7 +15647,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H168" s="9" t="s">
         <v>30</v>
       </c>
@@ -15658,7 +15658,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="169" spans="1:10" ht="57" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A169" s="9">
         <f>SUBTOTAL(3,$E$2:E169)</f>
         <v>31</v>
@@ -15686,7 +15686,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H170" s="12" t="s">
         <v>22</v>
       </c>
@@ -15697,7 +15697,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H171" s="12" t="s">
         <v>23</v>
       </c>
@@ -15708,7 +15708,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H172" s="12" t="s">
         <v>25</v>
       </c>
@@ -15719,7 +15719,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="173" spans="1:10" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H173" s="12" t="s">
         <v>28</v>
       </c>
@@ -15730,7 +15730,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="174" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A174" s="30"/>
       <c r="B174" s="30"/>
       <c r="C174" s="30"/>
@@ -15748,7 +15748,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A175" s="9">
         <f>SUBTOTAL(3,$E$2:E175)</f>
         <v>32</v>
@@ -15777,7 +15777,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H176" s="9" t="s">
         <v>22</v>
       </c>
@@ -15788,7 +15788,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H177" s="9" t="s">
         <v>23</v>
       </c>
@@ -15799,7 +15799,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H178" s="9" t="s">
         <v>25</v>
       </c>
@@ -15810,7 +15810,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="179" spans="1:10" ht="156.75" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:10" ht="151.80000000000001" x14ac:dyDescent="0.25">
       <c r="H179" s="9" t="s">
         <v>28</v>
       </c>
@@ -15821,7 +15821,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="180" spans="1:10" ht="156.75" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:10" ht="151.80000000000001" x14ac:dyDescent="0.25">
       <c r="H180" s="9" t="s">
         <v>30</v>
       </c>
@@ -15832,7 +15832,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="181" spans="1:10" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A181" s="9">
         <f>SUBTOTAL(3,$E$2:E181)</f>
         <v>33</v>
@@ -15861,7 +15861,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H182" s="9" t="s">
         <v>22</v>
       </c>
@@ -15872,7 +15872,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H183" s="9" t="s">
         <v>23</v>
       </c>
@@ -15883,7 +15883,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H184" s="9" t="s">
         <v>25</v>
       </c>
@@ -15894,7 +15894,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="185" spans="1:10" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H185" s="9" t="s">
         <v>28</v>
       </c>
@@ -15905,7 +15905,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="186" spans="1:10" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A186" s="9">
         <f>SUBTOTAL(3,$E$2:E186)</f>
         <v>34</v>
@@ -15934,7 +15934,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H187" s="9" t="s">
         <v>22</v>
       </c>
@@ -15945,7 +15945,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H188" s="9" t="s">
         <v>23</v>
       </c>
@@ -15956,7 +15956,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H189" s="9" t="s">
         <v>25</v>
       </c>
@@ -15967,7 +15967,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="190" spans="1:10" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H190" s="9" t="s">
         <v>28</v>
       </c>
@@ -15978,7 +15978,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="191" spans="1:10" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H191" s="9" t="s">
         <v>30</v>
       </c>
@@ -15989,7 +15989,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H192" s="9" t="s">
         <v>32</v>
       </c>
@@ -16000,7 +16000,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="193" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A193" s="9">
         <f>SUBTOTAL(3,$E$2:E193)</f>
         <v>35</v>
@@ -16029,7 +16029,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="194" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H194" s="9" t="s">
         <v>22</v>
       </c>
@@ -16040,7 +16040,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="195" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H195" s="9" t="s">
         <v>23</v>
       </c>
@@ -16051,7 +16051,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="196" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H196" s="9" t="s">
         <v>25</v>
       </c>
@@ -16062,7 +16062,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="197" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H197" s="9" t="s">
         <v>28</v>
       </c>
@@ -16073,7 +16073,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="198" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H198" s="9" t="s">
         <v>30</v>
       </c>
@@ -16084,7 +16084,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="199" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A199" s="9">
         <f>SUBTOTAL(3,$E$2:E199)</f>
         <v>36</v>
@@ -16112,7 +16112,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="200" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H200" s="12" t="s">
         <v>22</v>
       </c>
@@ -16123,7 +16123,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="201" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H201" s="12" t="s">
         <v>23</v>
       </c>
@@ -16134,7 +16134,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="202" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H202" s="12" t="s">
         <v>25</v>
       </c>
@@ -16145,7 +16145,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="203" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H203" s="12" t="s">
         <v>28</v>
       </c>
@@ -16156,7 +16156,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="204" spans="1:93" ht="15" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:93" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A204" s="30"/>
       <c r="B204" s="30"/>
       <c r="C204" s="30"/>
@@ -16174,7 +16174,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="205" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A205" s="9">
         <f>SUBTOTAL(3,$E$2:E205)</f>
         <v>37</v>
@@ -16283,7 +16283,7 @@
       <c r="CN205" s="13"/>
       <c r="CO205" s="13"/>
     </row>
-    <row r="206" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A206" s="9"/>
       <c r="B206" s="9"/>
       <c r="C206" s="10"/>
@@ -16381,7 +16381,7 @@
       <c r="CN206" s="13"/>
       <c r="CO206" s="13"/>
     </row>
-    <row r="207" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A207" s="9"/>
       <c r="B207" s="9"/>
       <c r="C207" s="10"/>
@@ -16479,7 +16479,7 @@
       <c r="CN207" s="13"/>
       <c r="CO207" s="13"/>
     </row>
-    <row r="208" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A208" s="9"/>
       <c r="B208" s="9"/>
       <c r="C208" s="10"/>
@@ -16577,7 +16577,7 @@
       <c r="CN208" s="13"/>
       <c r="CO208" s="13"/>
     </row>
-    <row r="209" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A209" s="9"/>
       <c r="B209" s="9"/>
       <c r="C209" s="10"/>
@@ -16675,7 +16675,7 @@
       <c r="CN209" s="13"/>
       <c r="CO209" s="13"/>
     </row>
-    <row r="210" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A210" s="9">
         <f>SUBTOTAL(3,$E$2:E210)</f>
         <v>38</v>
@@ -16784,7 +16784,7 @@
       <c r="CN210" s="13"/>
       <c r="CO210" s="13"/>
     </row>
-    <row r="211" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A211" s="9"/>
       <c r="B211" s="9"/>
       <c r="C211" s="10"/>
@@ -16882,7 +16882,7 @@
       <c r="CN211" s="13"/>
       <c r="CO211" s="13"/>
     </row>
-    <row r="212" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A212" s="9"/>
       <c r="B212" s="9"/>
       <c r="C212" s="10"/>
@@ -16980,7 +16980,7 @@
       <c r="CN212" s="13"/>
       <c r="CO212" s="13"/>
     </row>
-    <row r="213" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A213" s="9"/>
       <c r="B213" s="9"/>
       <c r="C213" s="10"/>
@@ -17078,7 +17078,7 @@
       <c r="CN213" s="13"/>
       <c r="CO213" s="13"/>
     </row>
-    <row r="214" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A214" s="9"/>
       <c r="B214" s="9"/>
       <c r="C214" s="10"/>
@@ -17176,7 +17176,7 @@
       <c r="CN214" s="13"/>
       <c r="CO214" s="13"/>
     </row>
-    <row r="215" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A215" s="9"/>
       <c r="B215" s="9"/>
       <c r="C215" s="10"/>
@@ -17275,7 +17275,7 @@
       <c r="CN215" s="13"/>
       <c r="CO215" s="13"/>
     </row>
-    <row r="216" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A216" s="9"/>
       <c r="B216" s="9"/>
       <c r="C216" s="10"/>
@@ -17374,7 +17374,7 @@
       <c r="CN216" s="13"/>
       <c r="CO216" s="13"/>
     </row>
-    <row r="217" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A217" s="9">
         <f>SUBTOTAL(3,$E$2:E217)</f>
         <v>39</v>
@@ -17483,7 +17483,7 @@
       <c r="CN217" s="13"/>
       <c r="CO217" s="13"/>
     </row>
-    <row r="218" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A218" s="9"/>
       <c r="B218" s="9"/>
       <c r="C218" s="10"/>
@@ -17581,7 +17581,7 @@
       <c r="CN218" s="13"/>
       <c r="CO218" s="13"/>
     </row>
-    <row r="219" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A219" s="9"/>
       <c r="B219" s="9"/>
       <c r="C219" s="10"/>
@@ -17679,7 +17679,7 @@
       <c r="CN219" s="13"/>
       <c r="CO219" s="13"/>
     </row>
-    <row r="220" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A220" s="9"/>
       <c r="B220" s="9"/>
       <c r="C220" s="10"/>
@@ -17777,7 +17777,7 @@
       <c r="CN220" s="13"/>
       <c r="CO220" s="13"/>
     </row>
-    <row r="221" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A221" s="9"/>
       <c r="B221" s="9"/>
       <c r="C221" s="10"/>
@@ -17875,7 +17875,7 @@
       <c r="CN221" s="13"/>
       <c r="CO221" s="13"/>
     </row>
-    <row r="222" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A222" s="9">
         <f>SUBTOTAL(3,$E$2:E222)</f>
         <v>40</v>
@@ -17984,7 +17984,7 @@
       <c r="CN222" s="13"/>
       <c r="CO222" s="13"/>
     </row>
-    <row r="223" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A223" s="9"/>
       <c r="B223" s="9"/>
       <c r="C223" s="10"/>
@@ -18082,7 +18082,7 @@
       <c r="CN223" s="13"/>
       <c r="CO223" s="13"/>
     </row>
-    <row r="224" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A224" s="9"/>
       <c r="B224" s="9"/>
       <c r="C224" s="10"/>
@@ -18180,7 +18180,7 @@
       <c r="CN224" s="13"/>
       <c r="CO224" s="13"/>
     </row>
-    <row r="225" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A225" s="9"/>
       <c r="B225" s="9"/>
       <c r="C225" s="10"/>
@@ -18278,7 +18278,7 @@
       <c r="CN225" s="13"/>
       <c r="CO225" s="13"/>
     </row>
-    <row r="226" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A226" s="9"/>
       <c r="B226" s="9"/>
       <c r="C226" s="10"/>
@@ -18376,7 +18376,7 @@
       <c r="CN226" s="13"/>
       <c r="CO226" s="13"/>
     </row>
-    <row r="227" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A227" s="9">
         <f>SUBTOTAL(3,$E$2:E227)</f>
         <v>41</v>
@@ -18485,7 +18485,7 @@
       <c r="CN227" s="13"/>
       <c r="CO227" s="13"/>
     </row>
-    <row r="228" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A228" s="9"/>
       <c r="B228" s="9"/>
       <c r="C228" s="10"/>
@@ -18583,7 +18583,7 @@
       <c r="CN228" s="13"/>
       <c r="CO228" s="13"/>
     </row>
-    <row r="229" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A229" s="9"/>
       <c r="B229" s="9"/>
       <c r="C229" s="10"/>
@@ -18681,7 +18681,7 @@
       <c r="CN229" s="13"/>
       <c r="CO229" s="13"/>
     </row>
-    <row r="230" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A230" s="9"/>
       <c r="B230" s="9"/>
       <c r="C230" s="10"/>
@@ -18779,7 +18779,7 @@
       <c r="CN230" s="13"/>
       <c r="CO230" s="13"/>
     </row>
-    <row r="231" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A231" s="23"/>
       <c r="B231" s="23"/>
       <c r="C231" s="24"/>
@@ -18880,7 +18880,7 @@
       <c r="CN231" s="13"/>
       <c r="CO231" s="13"/>
     </row>
-    <row r="232" spans="1:93" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:93" s="9" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A232" s="9">
         <f>SUBTOTAL(3,$E$2:E232)</f>
         <v>42</v>
@@ -18964,7 +18964,7 @@
       <c r="CN232" s="13"/>
       <c r="CO232" s="13"/>
     </row>
-    <row r="233" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B233" s="12"/>
       <c r="E233" s="9" t="s">
         <v>5</v>
@@ -19037,7 +19037,7 @@
       <c r="CN233" s="13"/>
       <c r="CO233" s="13"/>
     </row>
-    <row r="234" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B234" s="12"/>
       <c r="F234" s="12"/>
       <c r="G234" s="12"/>
@@ -19107,7 +19107,7 @@
       <c r="CN234" s="13"/>
       <c r="CO234" s="13"/>
     </row>
-    <row r="235" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B235" s="12"/>
       <c r="F235" s="12"/>
       <c r="G235" s="12"/>
@@ -19177,7 +19177,7 @@
       <c r="CN235" s="13"/>
       <c r="CO235" s="13"/>
     </row>
-    <row r="236" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B236" s="12"/>
       <c r="F236" s="12"/>
       <c r="G236" s="12"/>
@@ -19247,7 +19247,7 @@
       <c r="CN236" s="13"/>
       <c r="CO236" s="13"/>
     </row>
-    <row r="237" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A237" s="9">
         <f>SUBTOTAL(3,$E$2:E237)</f>
         <v>44</v>
@@ -19359,7 +19359,7 @@
       <c r="CN237" s="13"/>
       <c r="CO237" s="13"/>
     </row>
-    <row r="238" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H238" s="9" t="s">
         <v>22</v>
       </c>
@@ -19453,7 +19453,7 @@
       <c r="CN238" s="13"/>
       <c r="CO238" s="13"/>
     </row>
-    <row r="239" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H239" s="9" t="s">
         <v>23</v>
       </c>
@@ -19547,7 +19547,7 @@
       <c r="CN239" s="13"/>
       <c r="CO239" s="13"/>
     </row>
-    <row r="240" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H240" s="9" t="s">
         <v>25</v>
       </c>
@@ -19641,7 +19641,7 @@
       <c r="CN240" s="13"/>
       <c r="CO240" s="13"/>
     </row>
-    <row r="241" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H241" s="9" t="s">
         <v>28</v>
       </c>
@@ -19735,7 +19735,7 @@
       <c r="CN241" s="13"/>
       <c r="CO241" s="13"/>
     </row>
-    <row r="242" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H242" s="9" t="s">
         <v>30</v>
       </c>
@@ -19829,7 +19829,7 @@
       <c r="CN242" s="13"/>
       <c r="CO242" s="13"/>
     </row>
-    <row r="243" spans="1:93" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:93" s="9" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A243" s="9">
         <f>SUBTOTAL(3,$E$2:E243)</f>
         <v>45</v>
@@ -19913,7 +19913,7 @@
       <c r="CN243" s="13"/>
       <c r="CO243" s="13"/>
     </row>
-    <row r="244" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B244" s="12"/>
       <c r="F244" s="12"/>
       <c r="G244" s="12"/>
@@ -19983,7 +19983,7 @@
       <c r="CN244" s="13"/>
       <c r="CO244" s="13"/>
     </row>
-    <row r="245" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B245" s="12"/>
       <c r="F245" s="12"/>
       <c r="G245" s="12"/>
@@ -20053,7 +20053,7 @@
       <c r="CN245" s="13"/>
       <c r="CO245" s="13"/>
     </row>
-    <row r="246" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B246" s="12"/>
       <c r="F246" s="12"/>
       <c r="G246" s="12"/>
@@ -20123,7 +20123,7 @@
       <c r="CN246" s="13"/>
       <c r="CO246" s="13"/>
     </row>
-    <row r="247" spans="1:93" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:93" s="9" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B247" s="12"/>
       <c r="F247" s="12"/>
       <c r="G247" s="12"/>
@@ -20192,7 +20192,7 @@
       <c r="CN247" s="13"/>
       <c r="CO247" s="13"/>
     </row>
-    <row r="248" spans="1:93" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:93" s="9" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A248" s="9">
         <f>SUBTOTAL(3,$E$2:E248)</f>
         <v>46</v>
@@ -20276,7 +20276,7 @@
       <c r="CN248" s="13"/>
       <c r="CO248" s="13"/>
     </row>
-    <row r="249" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B249" s="12"/>
       <c r="F249" s="12"/>
       <c r="G249" s="12"/>
@@ -20346,7 +20346,7 @@
       <c r="CN249" s="13"/>
       <c r="CO249" s="13"/>
     </row>
-    <row r="250" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B250" s="12"/>
       <c r="F250" s="12"/>
       <c r="G250" s="12"/>
@@ -20416,7 +20416,7 @@
       <c r="CN250" s="13"/>
       <c r="CO250" s="13"/>
     </row>
-    <row r="251" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B251" s="12"/>
       <c r="F251" s="12"/>
       <c r="G251" s="12"/>
@@ -20486,7 +20486,7 @@
       <c r="CN251" s="13"/>
       <c r="CO251" s="13"/>
     </row>
-    <row r="252" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B252" s="12"/>
       <c r="F252" s="12"/>
       <c r="G252" s="12"/>
@@ -20556,7 +20556,7 @@
       <c r="CN252" s="13"/>
       <c r="CO252" s="13"/>
     </row>
-    <row r="253" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A253" s="23"/>
       <c r="B253" s="24"/>
       <c r="C253" s="23"/>
@@ -20630,7 +20630,7 @@
       <c r="CN253" s="13"/>
       <c r="CO253" s="13"/>
     </row>
-    <row r="254" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A254" s="9">
         <f>SUBTOTAL(3,$E$2:E254)</f>
         <v>47</v>
@@ -20742,7 +20742,7 @@
       <c r="CN254" s="13"/>
       <c r="CO254" s="13"/>
     </row>
-    <row r="255" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H255" s="9" t="s">
         <v>22</v>
       </c>
@@ -20836,7 +20836,7 @@
       <c r="CN255" s="13"/>
       <c r="CO255" s="13"/>
     </row>
-    <row r="256" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H256" s="9" t="s">
         <v>23</v>
       </c>
@@ -20930,7 +20930,7 @@
       <c r="CN256" s="13"/>
       <c r="CO256" s="13"/>
     </row>
-    <row r="257" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H257" s="9" t="s">
         <v>25</v>
       </c>
@@ -21024,7 +21024,7 @@
       <c r="CN257" s="13"/>
       <c r="CO257" s="13"/>
     </row>
-    <row r="258" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H258" s="9" t="s">
         <v>28</v>
       </c>
@@ -21118,7 +21118,7 @@
       <c r="CN258" s="13"/>
       <c r="CO258" s="13"/>
     </row>
-    <row r="259" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H259" s="9" t="s">
         <v>30</v>
       </c>
@@ -21212,7 +21212,7 @@
       <c r="CN259" s="13"/>
       <c r="CO259" s="13"/>
     </row>
-    <row r="260" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A260" s="9">
         <f>SUBTOTAL(3,$E$2:E260)</f>
         <v>48</v>
@@ -21324,7 +21324,7 @@
       <c r="CN260" s="13"/>
       <c r="CO260" s="13"/>
     </row>
-    <row r="261" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H261" s="9" t="s">
         <v>22</v>
       </c>
@@ -21418,7 +21418,7 @@
       <c r="CN261" s="13"/>
       <c r="CO261" s="13"/>
     </row>
-    <row r="262" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H262" s="9" t="s">
         <v>23</v>
       </c>
@@ -21512,7 +21512,7 @@
       <c r="CN262" s="13"/>
       <c r="CO262" s="13"/>
     </row>
-    <row r="263" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H263" s="9" t="s">
         <v>25</v>
       </c>
@@ -21606,7 +21606,7 @@
       <c r="CN263" s="13"/>
       <c r="CO263" s="13"/>
     </row>
-    <row r="264" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H264" s="9" t="s">
         <v>28</v>
       </c>
@@ -21700,7 +21700,7 @@
       <c r="CN264" s="13"/>
       <c r="CO264" s="13"/>
     </row>
-    <row r="265" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H265" s="9" t="s">
         <v>30</v>
       </c>
@@ -21794,7 +21794,7 @@
       <c r="CN265" s="13"/>
       <c r="CO265" s="13"/>
     </row>
-    <row r="266" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H266" s="9" t="s">
         <v>32</v>
       </c>
@@ -21888,7 +21888,7 @@
       <c r="CN266" s="13"/>
       <c r="CO266" s="13"/>
     </row>
-    <row r="267" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H267" s="9" t="s">
         <v>72</v>
       </c>
@@ -21982,7 +21982,7 @@
       <c r="CN267" s="13"/>
       <c r="CO267" s="13"/>
     </row>
-    <row r="268" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H268" s="9" t="s">
         <v>75</v>
       </c>
@@ -22076,7 +22076,7 @@
       <c r="CN268" s="13"/>
       <c r="CO268" s="13"/>
     </row>
-    <row r="269" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H269" s="9" t="s">
         <v>103</v>
       </c>
@@ -22170,7 +22170,7 @@
       <c r="CN269" s="13"/>
       <c r="CO269" s="13"/>
     </row>
-    <row r="270" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H270" s="9" t="s">
         <v>104</v>
       </c>
@@ -22264,7 +22264,7 @@
       <c r="CN270" s="13"/>
       <c r="CO270" s="13"/>
     </row>
-    <row r="271" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A271" s="9">
         <f>SUBTOTAL(3,$E$2:E271)</f>
         <v>49</v>
@@ -22376,7 +22376,7 @@
       <c r="CN271" s="13"/>
       <c r="CO271" s="13"/>
     </row>
-    <row r="272" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H272" s="9" t="s">
         <v>22</v>
       </c>
@@ -22470,7 +22470,7 @@
       <c r="CN272" s="13"/>
       <c r="CO272" s="13"/>
     </row>
-    <row r="273" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H273" s="9" t="s">
         <v>23</v>
       </c>
@@ -22564,7 +22564,7 @@
       <c r="CN273" s="13"/>
       <c r="CO273" s="13"/>
     </row>
-    <row r="274" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H274" s="9" t="s">
         <v>25</v>
       </c>
@@ -22658,7 +22658,7 @@
       <c r="CN274" s="13"/>
       <c r="CO274" s="13"/>
     </row>
-    <row r="275" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H275" s="9" t="s">
         <v>28</v>
       </c>
@@ -22752,7 +22752,7 @@
       <c r="CN275" s="13"/>
       <c r="CO275" s="13"/>
     </row>
-    <row r="276" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H276" s="9" t="s">
         <v>30</v>
       </c>
@@ -22846,7 +22846,7 @@
       <c r="CN276" s="13"/>
       <c r="CO276" s="13"/>
     </row>
-    <row r="277" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H277" s="9" t="s">
         <v>32</v>
       </c>
@@ -22940,7 +22940,7 @@
       <c r="CN277" s="13"/>
       <c r="CO277" s="13"/>
     </row>
-    <row r="278" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H278" s="9" t="s">
         <v>72</v>
       </c>
@@ -23034,7 +23034,7 @@
       <c r="CN278" s="13"/>
       <c r="CO278" s="13"/>
     </row>
-    <row r="279" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H279" s="9" t="s">
         <v>75</v>
       </c>
@@ -23128,7 +23128,7 @@
       <c r="CN279" s="13"/>
       <c r="CO279" s="13"/>
     </row>
-    <row r="280" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H280" s="9" t="s">
         <v>103</v>
       </c>
@@ -23222,7 +23222,7 @@
       <c r="CN280" s="13"/>
       <c r="CO280" s="13"/>
     </row>
-    <row r="281" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H281" s="9" t="s">
         <v>104</v>
       </c>
@@ -23316,7 +23316,7 @@
       <c r="CN281" s="13"/>
       <c r="CO281" s="13"/>
     </row>
-    <row r="282" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:93" x14ac:dyDescent="0.25">
       <c r="E282" s="12"/>
       <c r="H282" s="9" t="s">
         <v>105</v>
@@ -23411,7 +23411,7 @@
       <c r="CN282" s="13"/>
       <c r="CO282" s="13"/>
     </row>
-    <row r="283" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A283" s="9">
         <f>SUBTOTAL(3,$E$2:E283)</f>
         <v>50</v>
@@ -23523,7 +23523,7 @@
       <c r="CN283" s="13"/>
       <c r="CO283" s="13"/>
     </row>
-    <row r="284" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H284" s="9" t="s">
         <v>22</v>
       </c>
@@ -23617,7 +23617,7 @@
       <c r="CN284" s="13"/>
       <c r="CO284" s="13"/>
     </row>
-    <row r="285" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H285" s="9" t="s">
         <v>23</v>
       </c>
@@ -23711,7 +23711,7 @@
       <c r="CN285" s="13"/>
       <c r="CO285" s="13"/>
     </row>
-    <row r="286" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H286" s="9" t="s">
         <v>25</v>
       </c>
@@ -23805,7 +23805,7 @@
       <c r="CN286" s="13"/>
       <c r="CO286" s="13"/>
     </row>
-    <row r="287" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H287" s="9" t="s">
         <v>28</v>
       </c>
@@ -23899,7 +23899,7 @@
       <c r="CN287" s="13"/>
       <c r="CO287" s="13"/>
     </row>
-    <row r="288" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A288" s="24"/>
       <c r="B288" s="24"/>
       <c r="C288" s="24"/>
@@ -24000,7 +24000,7 @@
       <c r="CN288" s="13"/>
       <c r="CO288" s="13"/>
     </row>
-    <row r="289" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A289" s="9">
         <f>SUBTOTAL(3,$E$2:E289)</f>
         <v>51</v>
@@ -24111,7 +24111,7 @@
       <c r="CN289" s="13"/>
       <c r="CO289" s="13"/>
     </row>
-    <row r="290" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H290" s="12" t="s">
         <v>22</v>
       </c>
@@ -24205,7 +24205,7 @@
       <c r="CN290" s="13"/>
       <c r="CO290" s="13"/>
     </row>
-    <row r="291" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H291" s="12" t="s">
         <v>23</v>
       </c>
@@ -24299,7 +24299,7 @@
       <c r="CN291" s="13"/>
       <c r="CO291" s="13"/>
     </row>
-    <row r="292" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H292" s="12" t="s">
         <v>25</v>
       </c>
@@ -24393,7 +24393,7 @@
       <c r="CN292" s="13"/>
       <c r="CO292" s="13"/>
     </row>
-    <row r="293" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H293" s="12" t="s">
         <v>28</v>
       </c>
@@ -24487,7 +24487,7 @@
       <c r="CN293" s="13"/>
       <c r="CO293" s="13"/>
     </row>
-    <row r="294" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H294" s="12" t="s">
         <v>30</v>
       </c>
@@ -24581,7 +24581,7 @@
       <c r="CN294" s="13"/>
       <c r="CO294" s="13"/>
     </row>
-    <row r="295" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H295" s="12" t="s">
         <v>32</v>
       </c>
@@ -24675,7 +24675,7 @@
       <c r="CN295" s="13"/>
       <c r="CO295" s="13"/>
     </row>
-    <row r="296" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A296" s="9">
         <f>SUBTOTAL(3,$E$2:E296)</f>
         <v>52</v>
@@ -24785,7 +24785,7 @@
       <c r="CN296" s="13"/>
       <c r="CO296" s="13"/>
     </row>
-    <row r="297" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H297" s="12" t="s">
         <v>22</v>
       </c>
@@ -24879,7 +24879,7 @@
       <c r="CN297" s="13"/>
       <c r="CO297" s="13"/>
     </row>
-    <row r="298" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H298" s="12" t="s">
         <v>23</v>
       </c>
@@ -24973,7 +24973,7 @@
       <c r="CN298" s="13"/>
       <c r="CO298" s="13"/>
     </row>
-    <row r="299" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H299" s="12" t="s">
         <v>25</v>
       </c>
@@ -25067,7 +25067,7 @@
       <c r="CN299" s="13"/>
       <c r="CO299" s="13"/>
     </row>
-    <row r="300" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H300" s="12" t="s">
         <v>28</v>
       </c>
@@ -25161,7 +25161,7 @@
       <c r="CN300" s="13"/>
       <c r="CO300" s="13"/>
     </row>
-    <row r="301" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H301" s="12" t="s">
         <v>30</v>
       </c>
@@ -25255,7 +25255,7 @@
       <c r="CN301" s="13"/>
       <c r="CO301" s="13"/>
     </row>
-    <row r="302" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H302" s="12" t="s">
         <v>32</v>
       </c>
@@ -25349,7 +25349,7 @@
       <c r="CN302" s="13"/>
       <c r="CO302" s="13"/>
     </row>
-    <row r="303" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A303" s="9">
         <f>SUBTOTAL(3,$E$2:E303)</f>
         <v>53</v>
@@ -25460,7 +25460,7 @@
       <c r="CN303" s="13"/>
       <c r="CO303" s="13"/>
     </row>
-    <row r="304" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H304" s="12" t="s">
         <v>22</v>
       </c>
@@ -25554,7 +25554,7 @@
       <c r="CN304" s="13"/>
       <c r="CO304" s="13"/>
     </row>
-    <row r="305" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H305" s="12" t="s">
         <v>23</v>
       </c>
@@ -25648,7 +25648,7 @@
       <c r="CN305" s="13"/>
       <c r="CO305" s="13"/>
     </row>
-    <row r="306" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H306" s="12" t="s">
         <v>25</v>
       </c>
@@ -25742,7 +25742,7 @@
       <c r="CN306" s="13"/>
       <c r="CO306" s="13"/>
     </row>
-    <row r="307" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H307" s="12" t="s">
         <v>28</v>
       </c>
@@ -25836,7 +25836,7 @@
       <c r="CN307" s="13"/>
       <c r="CO307" s="13"/>
     </row>
-    <row r="308" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H308" s="12" t="s">
         <v>30</v>
       </c>
@@ -25930,7 +25930,7 @@
       <c r="CN308" s="13"/>
       <c r="CO308" s="13"/>
     </row>
-    <row r="309" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A309" s="9">
         <f>SUBTOTAL(3,$E$2:E309)</f>
         <v>54</v>
@@ -26041,7 +26041,7 @@
       <c r="CN309" s="13"/>
       <c r="CO309" s="13"/>
     </row>
-    <row r="310" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H310" s="12" t="s">
         <v>22</v>
       </c>
@@ -26135,7 +26135,7 @@
       <c r="CN310" s="13"/>
       <c r="CO310" s="13"/>
     </row>
-    <row r="311" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H311" s="12" t="s">
         <v>23</v>
       </c>
@@ -26229,7 +26229,7 @@
       <c r="CN311" s="13"/>
       <c r="CO311" s="13"/>
     </row>
-    <row r="312" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H312" s="12" t="s">
         <v>25</v>
       </c>
@@ -26323,7 +26323,7 @@
       <c r="CN312" s="13"/>
       <c r="CO312" s="13"/>
     </row>
-    <row r="313" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H313" s="12" t="s">
         <v>28</v>
       </c>
@@ -26417,7 +26417,7 @@
       <c r="CN313" s="13"/>
       <c r="CO313" s="13"/>
     </row>
-    <row r="314" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H314" s="12" t="s">
         <v>30</v>
       </c>
@@ -26511,7 +26511,7 @@
       <c r="CN314" s="13"/>
       <c r="CO314" s="13"/>
     </row>
-    <row r="315" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H315" s="12" t="s">
         <v>32</v>
       </c>
@@ -26605,7 +26605,7 @@
       <c r="CN315" s="13"/>
       <c r="CO315" s="13"/>
     </row>
-    <row r="316" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A316" s="9">
         <f>SUBTOTAL(3,$E$2:E316)</f>
         <v>55</v>
@@ -26716,7 +26716,7 @@
       <c r="CN316" s="13"/>
       <c r="CO316" s="13"/>
     </row>
-    <row r="317" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H317" s="12" t="s">
         <v>22</v>
       </c>
@@ -26810,7 +26810,7 @@
       <c r="CN317" s="13"/>
       <c r="CO317" s="13"/>
     </row>
-    <row r="318" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H318" s="12" t="s">
         <v>23</v>
       </c>
@@ -26904,7 +26904,7 @@
       <c r="CN318" s="13"/>
       <c r="CO318" s="13"/>
     </row>
-    <row r="319" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H319" s="12" t="s">
         <v>25</v>
       </c>
@@ -26998,7 +26998,7 @@
       <c r="CN319" s="13"/>
       <c r="CO319" s="13"/>
     </row>
-    <row r="320" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H320" s="12" t="s">
         <v>28</v>
       </c>
@@ -27092,7 +27092,7 @@
       <c r="CN320" s="13"/>
       <c r="CO320" s="13"/>
     </row>
-    <row r="321" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H321" s="12" t="s">
         <v>30</v>
       </c>
@@ -27186,7 +27186,7 @@
       <c r="CN321" s="13"/>
       <c r="CO321" s="13"/>
     </row>
-    <row r="322" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H322" s="12" t="s">
         <v>32</v>
       </c>
@@ -27280,7 +27280,7 @@
       <c r="CN322" s="13"/>
       <c r="CO322" s="13"/>
     </row>
-    <row r="323" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H323" s="12" t="s">
         <v>72</v>
       </c>
@@ -27374,7 +27374,7 @@
       <c r="CN323" s="13"/>
       <c r="CO323" s="13"/>
     </row>
-    <row r="324" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A324" s="9">
         <f>SUBTOTAL(3,$E$2:E324)</f>
         <v>56</v>
@@ -27485,7 +27485,7 @@
       <c r="CN324" s="13"/>
       <c r="CO324" s="13"/>
     </row>
-    <row r="325" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H325" s="12" t="s">
         <v>22</v>
       </c>
@@ -27579,7 +27579,7 @@
       <c r="CN325" s="13"/>
       <c r="CO325" s="13"/>
     </row>
-    <row r="326" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H326" s="12" t="s">
         <v>23</v>
       </c>
@@ -27673,7 +27673,7 @@
       <c r="CN326" s="13"/>
       <c r="CO326" s="13"/>
     </row>
-    <row r="327" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H327" s="12" t="s">
         <v>25</v>
       </c>
@@ -27767,7 +27767,7 @@
       <c r="CN327" s="13"/>
       <c r="CO327" s="13"/>
     </row>
-    <row r="328" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H328" s="12" t="s">
         <v>28</v>
       </c>
@@ -27861,7 +27861,7 @@
       <c r="CN328" s="13"/>
       <c r="CO328" s="13"/>
     </row>
-    <row r="329" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H329" s="12" t="s">
         <v>30</v>
       </c>
@@ -27955,7 +27955,7 @@
       <c r="CN329" s="13"/>
       <c r="CO329" s="13"/>
     </row>
-    <row r="330" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H330" s="12" t="s">
         <v>32</v>
       </c>
@@ -28049,7 +28049,7 @@
       <c r="CN330" s="13"/>
       <c r="CO330" s="13"/>
     </row>
-    <row r="331" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A331" s="9">
         <f>SUBTOTAL(3,$E$2:E331)</f>
         <v>57</v>
@@ -28160,7 +28160,7 @@
       <c r="CN331" s="13"/>
       <c r="CO331" s="13"/>
     </row>
-    <row r="332" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H332" s="12" t="s">
         <v>22</v>
       </c>
@@ -28254,7 +28254,7 @@
       <c r="CN332" s="13"/>
       <c r="CO332" s="13"/>
     </row>
-    <row r="333" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H333" s="12" t="s">
         <v>23</v>
       </c>
@@ -28348,7 +28348,7 @@
       <c r="CN333" s="13"/>
       <c r="CO333" s="13"/>
     </row>
-    <row r="334" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H334" s="12" t="s">
         <v>25</v>
       </c>
@@ -28442,7 +28442,7 @@
       <c r="CN334" s="13"/>
       <c r="CO334" s="13"/>
     </row>
-    <row r="335" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H335" s="12" t="s">
         <v>28</v>
       </c>
@@ -28536,7 +28536,7 @@
       <c r="CN335" s="13"/>
       <c r="CO335" s="13"/>
     </row>
-    <row r="336" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H336" s="12" t="s">
         <v>30</v>
       </c>
@@ -28630,7 +28630,7 @@
       <c r="CN336" s="13"/>
       <c r="CO336" s="13"/>
     </row>
-    <row r="337" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H337" s="12" t="s">
         <v>32</v>
       </c>
@@ -28724,7 +28724,7 @@
       <c r="CN337" s="13"/>
       <c r="CO337" s="13"/>
     </row>
-    <row r="338" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H338" s="12" t="s">
         <v>72</v>
       </c>
@@ -28818,7 +28818,7 @@
       <c r="CN338" s="13"/>
       <c r="CO338" s="13"/>
     </row>
-    <row r="339" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H339" s="12" t="s">
         <v>75</v>
       </c>
@@ -28912,7 +28912,7 @@
       <c r="CN339" s="13"/>
       <c r="CO339" s="13"/>
     </row>
-    <row r="340" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A340" s="9">
         <f>SUBTOTAL(3,$E$2:E340)</f>
         <v>58</v>
@@ -29023,7 +29023,7 @@
       <c r="CN340" s="13"/>
       <c r="CO340" s="13"/>
     </row>
-    <row r="341" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H341" s="12" t="s">
         <v>22</v>
       </c>
@@ -29117,7 +29117,7 @@
       <c r="CN341" s="13"/>
       <c r="CO341" s="13"/>
     </row>
-    <row r="342" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H342" s="12" t="s">
         <v>23</v>
       </c>
@@ -29211,7 +29211,7 @@
       <c r="CN342" s="13"/>
       <c r="CO342" s="13"/>
     </row>
-    <row r="343" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H343" s="12" t="s">
         <v>25</v>
       </c>
@@ -29305,7 +29305,7 @@
       <c r="CN343" s="13"/>
       <c r="CO343" s="13"/>
     </row>
-    <row r="344" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H344" s="12" t="s">
         <v>28</v>
       </c>
@@ -29399,7 +29399,7 @@
       <c r="CN344" s="13"/>
       <c r="CO344" s="13"/>
     </row>
-    <row r="345" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H345" s="12" t="s">
         <v>30</v>
       </c>
@@ -29493,7 +29493,7 @@
       <c r="CN345" s="13"/>
       <c r="CO345" s="13"/>
     </row>
-    <row r="346" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H346" s="12" t="s">
         <v>32</v>
       </c>
@@ -29587,7 +29587,7 @@
       <c r="CN346" s="13"/>
       <c r="CO346" s="13"/>
     </row>
-    <row r="347" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H347" s="12" t="s">
         <v>72</v>
       </c>
@@ -29681,7 +29681,7 @@
       <c r="CN347" s="13"/>
       <c r="CO347" s="13"/>
     </row>
-    <row r="348" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H348" s="12" t="s">
         <v>75</v>
       </c>
@@ -29775,7 +29775,7 @@
       <c r="CN348" s="13"/>
       <c r="CO348" s="13"/>
     </row>
-    <row r="349" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A349" s="9">
         <f>SUBTOTAL(3,$E$2:E349)</f>
         <v>59</v>
@@ -29886,7 +29886,7 @@
       <c r="CN349" s="13"/>
       <c r="CO349" s="13"/>
     </row>
-    <row r="350" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H350" s="12" t="s">
         <v>22</v>
       </c>
@@ -29980,7 +29980,7 @@
       <c r="CN350" s="13"/>
       <c r="CO350" s="13"/>
     </row>
-    <row r="351" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H351" s="12" t="s">
         <v>23</v>
       </c>
@@ -30074,7 +30074,7 @@
       <c r="CN351" s="13"/>
       <c r="CO351" s="13"/>
     </row>
-    <row r="352" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H352" s="12" t="s">
         <v>25</v>
       </c>
@@ -30168,7 +30168,7 @@
       <c r="CN352" s="13"/>
       <c r="CO352" s="13"/>
     </row>
-    <row r="353" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A353" s="9">
         <f>SUBTOTAL(3,$E$2:E353)</f>
         <v>60</v>
@@ -30279,7 +30279,7 @@
       <c r="CN353" s="13"/>
       <c r="CO353" s="13"/>
     </row>
-    <row r="354" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H354" s="12" t="s">
         <v>22</v>
       </c>
@@ -30373,7 +30373,7 @@
       <c r="CN354" s="13"/>
       <c r="CO354" s="13"/>
     </row>
-    <row r="355" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H355" s="12" t="s">
         <v>23</v>
       </c>
@@ -30467,7 +30467,7 @@
       <c r="CN355" s="13"/>
       <c r="CO355" s="13"/>
     </row>
-    <row r="356" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H356" s="12" t="s">
         <v>25</v>
       </c>
@@ -30561,7 +30561,7 @@
       <c r="CN356" s="13"/>
       <c r="CO356" s="13"/>
     </row>
-    <row r="357" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A357" s="9">
         <f>SUBTOTAL(3,$E$2:E357)</f>
         <v>61</v>
@@ -30672,7 +30672,7 @@
       <c r="CN357" s="13"/>
       <c r="CO357" s="13"/>
     </row>
-    <row r="358" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H358" s="12" t="s">
         <v>22</v>
       </c>
@@ -30766,7 +30766,7 @@
       <c r="CN358" s="13"/>
       <c r="CO358" s="13"/>
     </row>
-    <row r="359" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H359" s="12" t="s">
         <v>23</v>
       </c>
@@ -30860,7 +30860,7 @@
       <c r="CN359" s="13"/>
       <c r="CO359" s="13"/>
     </row>
-    <row r="360" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H360" s="12" t="s">
         <v>25</v>
       </c>
@@ -30954,7 +30954,7 @@
       <c r="CN360" s="13"/>
       <c r="CO360" s="13"/>
     </row>
-    <row r="361" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H361" s="12" t="s">
         <v>28</v>
       </c>
@@ -31048,7 +31048,7 @@
       <c r="CN361" s="13"/>
       <c r="CO361" s="13"/>
     </row>
-    <row r="362" spans="1:93" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:93" ht="69" x14ac:dyDescent="0.25">
       <c r="A362" s="9">
         <f>SUBTOTAL(3,$E$2:E362)</f>
         <v>62</v>
@@ -31159,7 +31159,7 @@
       <c r="CN362" s="13"/>
       <c r="CO362" s="13"/>
     </row>
-    <row r="363" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H363" s="12" t="s">
         <v>22</v>
       </c>
@@ -31253,7 +31253,7 @@
       <c r="CN363" s="13"/>
       <c r="CO363" s="13"/>
     </row>
-    <row r="364" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H364" s="12" t="s">
         <v>23</v>
       </c>
@@ -31347,7 +31347,7 @@
       <c r="CN364" s="13"/>
       <c r="CO364" s="13"/>
     </row>
-    <row r="365" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H365" s="12" t="s">
         <v>25</v>
       </c>
@@ -31441,7 +31441,7 @@
       <c r="CN365" s="13"/>
       <c r="CO365" s="13"/>
     </row>
-    <row r="366" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A366" s="9">
         <f>SUBTOTAL(3,$E$2:E366)</f>
         <v>63</v>
@@ -31552,7 +31552,7 @@
       <c r="CN366" s="13"/>
       <c r="CO366" s="13"/>
     </row>
-    <row r="367" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H367" s="12" t="s">
         <v>22</v>
       </c>
@@ -31646,7 +31646,7 @@
       <c r="CN367" s="13"/>
       <c r="CO367" s="13"/>
     </row>
-    <row r="368" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H368" s="12" t="s">
         <v>23</v>
       </c>
@@ -31740,7 +31740,7 @@
       <c r="CN368" s="13"/>
       <c r="CO368" s="13"/>
     </row>
-    <row r="369" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H369" s="12" t="s">
         <v>25</v>
       </c>
@@ -31834,7 +31834,7 @@
       <c r="CN369" s="13"/>
       <c r="CO369" s="13"/>
     </row>
-    <row r="370" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H370" s="12" t="s">
         <v>28</v>
       </c>
@@ -31928,7 +31928,7 @@
       <c r="CN370" s="13"/>
       <c r="CO370" s="13"/>
     </row>
-    <row r="371" spans="1:93" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:93" s="9" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A371" s="9">
         <f>SUBTOTAL(3,$E$2:E371)</f>
         <v>64</v>
@@ -32013,7 +32013,7 @@
       <c r="CN371" s="13"/>
       <c r="CO371" s="13"/>
     </row>
-    <row r="372" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H372" s="12" t="s">
         <v>22</v>
       </c>
@@ -32107,7 +32107,7 @@
       <c r="CN372" s="13"/>
       <c r="CO372" s="13"/>
     </row>
-    <row r="373" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H373" s="12" t="s">
         <v>23</v>
       </c>
@@ -32201,7 +32201,7 @@
       <c r="CN373" s="13"/>
       <c r="CO373" s="13"/>
     </row>
-    <row r="374" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H374" s="12" t="s">
         <v>25</v>
       </c>
@@ -32295,7 +32295,7 @@
       <c r="CN374" s="13"/>
       <c r="CO374" s="13"/>
     </row>
-    <row r="375" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H375" s="12" t="s">
         <v>28</v>
       </c>
@@ -32389,7 +32389,7 @@
       <c r="CN375" s="13"/>
       <c r="CO375" s="13"/>
     </row>
-    <row r="376" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H376" s="12" t="s">
         <v>30</v>
       </c>
@@ -32483,7 +32483,7 @@
       <c r="CN376" s="13"/>
       <c r="CO376" s="13"/>
     </row>
-    <row r="377" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A377" s="9">
         <f>SUBTOTAL(3,$E$2:E377)</f>
         <v>65</v>
@@ -32594,7 +32594,7 @@
       <c r="CN377" s="13"/>
       <c r="CO377" s="13"/>
     </row>
-    <row r="378" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H378" s="12" t="s">
         <v>22</v>
       </c>
@@ -32688,7 +32688,7 @@
       <c r="CN378" s="13"/>
       <c r="CO378" s="13"/>
     </row>
-    <row r="379" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H379" s="12" t="s">
         <v>23</v>
       </c>
@@ -32782,7 +32782,7 @@
       <c r="CN379" s="13"/>
       <c r="CO379" s="13"/>
     </row>
-    <row r="380" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H380" s="12" t="s">
         <v>25</v>
       </c>
@@ -32876,7 +32876,7 @@
       <c r="CN380" s="13"/>
       <c r="CO380" s="13"/>
     </row>
-    <row r="381" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H381" s="12" t="s">
         <v>28</v>
       </c>
@@ -32970,7 +32970,7 @@
       <c r="CN381" s="13"/>
       <c r="CO381" s="13"/>
     </row>
-    <row r="382" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A382" s="9">
         <f>SUBTOTAL(3,$E$2:E382)</f>
         <v>66</v>
@@ -33081,7 +33081,7 @@
       <c r="CN382" s="13"/>
       <c r="CO382" s="13"/>
     </row>
-    <row r="383" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H383" s="12" t="s">
         <v>22</v>
       </c>
@@ -33175,7 +33175,7 @@
       <c r="CN383" s="13"/>
       <c r="CO383" s="13"/>
     </row>
-    <row r="384" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H384" s="12" t="s">
         <v>23</v>
       </c>
@@ -33269,7 +33269,7 @@
       <c r="CN384" s="13"/>
       <c r="CO384" s="13"/>
     </row>
-    <row r="385" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:93" ht="41.4" x14ac:dyDescent="0.25">
       <c r="H385" s="12" t="s">
         <v>25</v>
       </c>
@@ -33363,7 +33363,7 @@
       <c r="CN385" s="13"/>
       <c r="CO385" s="13"/>
     </row>
-    <row r="386" spans="1:93" s="26" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:93" s="26" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A386" s="12"/>
       <c r="B386" s="12"/>
       <c r="C386" s="12"/>
@@ -33464,7 +33464,7 @@
       <c r="CN386" s="13"/>
       <c r="CO386" s="13"/>
     </row>
-    <row r="387" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A387" s="9">
         <f>SUBTOTAL(3,$E$2:E387)</f>
         <v>67</v>
@@ -33575,7 +33575,7 @@
       <c r="CN387" s="13"/>
       <c r="CO387" s="13"/>
     </row>
-    <row r="388" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H388" s="12" t="s">
         <v>22</v>
       </c>
@@ -33669,7 +33669,7 @@
       <c r="CN388" s="13"/>
       <c r="CO388" s="13"/>
     </row>
-    <row r="389" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H389" s="12" t="s">
         <v>23</v>
       </c>
@@ -33763,7 +33763,7 @@
       <c r="CN389" s="13"/>
       <c r="CO389" s="13"/>
     </row>
-    <row r="390" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A390" s="26"/>
       <c r="B390" s="26"/>
       <c r="C390" s="26"/>
@@ -33864,7 +33864,7 @@
       <c r="CN390" s="13"/>
       <c r="CO390" s="13"/>
     </row>
-    <row r="391" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A391" s="9">
         <f>SUBTOTAL(3,$E$2:E391)</f>
         <v>68</v>
@@ -33975,7 +33975,7 @@
       <c r="CN391" s="13"/>
       <c r="CO391" s="13"/>
     </row>
-    <row r="392" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H392" s="12" t="s">
         <v>22</v>
       </c>
@@ -34069,7 +34069,7 @@
       <c r="CN392" s="13"/>
       <c r="CO392" s="13"/>
     </row>
-    <row r="393" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H393" s="12" t="s">
         <v>23</v>
       </c>
@@ -34163,7 +34163,7 @@
       <c r="CN393" s="13"/>
       <c r="CO393" s="13"/>
     </row>
-    <row r="394" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H394" s="12" t="s">
         <v>25</v>
       </c>
@@ -34257,7 +34257,7 @@
       <c r="CN394" s="13"/>
       <c r="CO394" s="13"/>
     </row>
-    <row r="395" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H395" s="12" t="s">
         <v>28</v>
       </c>
@@ -34351,7 +34351,7 @@
       <c r="CN395" s="13"/>
       <c r="CO395" s="13"/>
     </row>
-    <row r="396" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H396" s="12" t="s">
         <v>30</v>
       </c>
@@ -34445,7 +34445,7 @@
       <c r="CN396" s="13"/>
       <c r="CO396" s="13"/>
     </row>
-    <row r="397" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A397" s="9">
         <f>SUBTOTAL(3,$E$2:E397)</f>
         <v>69</v>
@@ -34556,7 +34556,7 @@
       <c r="CN397" s="13"/>
       <c r="CO397" s="13"/>
     </row>
-    <row r="398" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H398" s="12" t="s">
         <v>22</v>
       </c>
@@ -34650,7 +34650,7 @@
       <c r="CN398" s="13"/>
       <c r="CO398" s="13"/>
     </row>
-    <row r="399" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H399" s="12" t="s">
         <v>23</v>
       </c>
@@ -34744,7 +34744,7 @@
       <c r="CN399" s="13"/>
       <c r="CO399" s="13"/>
     </row>
-    <row r="400" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H400" s="12" t="s">
         <v>25</v>
       </c>
@@ -34838,7 +34838,7 @@
       <c r="CN400" s="13"/>
       <c r="CO400" s="13"/>
     </row>
-    <row r="401" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H401" s="12" t="s">
         <v>28</v>
       </c>
@@ -34932,7 +34932,7 @@
       <c r="CN401" s="13"/>
       <c r="CO401" s="13"/>
     </row>
-    <row r="402" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H402" s="12" t="s">
         <v>30</v>
       </c>
@@ -35026,7 +35026,7 @@
       <c r="CN402" s="13"/>
       <c r="CO402" s="13"/>
     </row>
-    <row r="403" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H403" s="12" t="s">
         <v>32</v>
       </c>
@@ -35120,7 +35120,7 @@
       <c r="CN403" s="13"/>
       <c r="CO403" s="13"/>
     </row>
-    <row r="404" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A404" s="9">
         <f>SUBTOTAL(3,$E$2:E404)</f>
         <v>70</v>
@@ -35231,7 +35231,7 @@
       <c r="CN404" s="13"/>
       <c r="CO404" s="13"/>
     </row>
-    <row r="405" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H405" s="12" t="s">
         <v>22</v>
       </c>
@@ -35325,7 +35325,7 @@
       <c r="CN405" s="13"/>
       <c r="CO405" s="13"/>
     </row>
-    <row r="406" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H406" s="12" t="s">
         <v>23</v>
       </c>
@@ -35419,7 +35419,7 @@
       <c r="CN406" s="13"/>
       <c r="CO406" s="13"/>
     </row>
-    <row r="407" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H407" s="12" t="s">
         <v>25</v>
       </c>
@@ -35513,7 +35513,7 @@
       <c r="CN407" s="13"/>
       <c r="CO407" s="13"/>
     </row>
-    <row r="408" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H408" s="12" t="s">
         <v>28</v>
       </c>
@@ -35607,7 +35607,7 @@
       <c r="CN408" s="13"/>
       <c r="CO408" s="13"/>
     </row>
-    <row r="409" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H409" s="12" t="s">
         <v>30</v>
       </c>
@@ -35701,7 +35701,7 @@
       <c r="CN409" s="13"/>
       <c r="CO409" s="13"/>
     </row>
-    <row r="410" spans="1:93" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H410" s="12" t="s">
         <v>32</v>
       </c>
@@ -35795,7 +35795,7 @@
       <c r="CN410" s="13"/>
       <c r="CO410" s="13"/>
     </row>
-    <row r="411" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H411" s="12" t="s">
         <v>72</v>
       </c>
@@ -35889,7 +35889,7 @@
       <c r="CN411" s="13"/>
       <c r="CO411" s="13"/>
     </row>
-    <row r="412" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H412" s="12" t="s">
         <v>75</v>
       </c>
@@ -35983,7 +35983,7 @@
       <c r="CN412" s="13"/>
       <c r="CO412" s="13"/>
     </row>
-    <row r="413" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H413" s="12" t="s">
         <v>103</v>
       </c>
@@ -36077,7 +36077,7 @@
       <c r="CN413" s="13"/>
       <c r="CO413" s="13"/>
     </row>
-    <row r="414" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A414" s="9">
         <f>SUBTOTAL(3,$E$2:E414)</f>
         <v>71</v>
@@ -36188,7 +36188,7 @@
       <c r="CN414" s="13"/>
       <c r="CO414" s="13"/>
     </row>
-    <row r="415" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H415" s="12" t="s">
         <v>22</v>
       </c>
@@ -36282,7 +36282,7 @@
       <c r="CN415" s="13"/>
       <c r="CO415" s="13"/>
     </row>
-    <row r="416" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H416" s="12" t="s">
         <v>23</v>
       </c>
@@ -36376,7 +36376,7 @@
       <c r="CN416" s="13"/>
       <c r="CO416" s="13"/>
     </row>
-    <row r="417" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H417" s="12" t="s">
         <v>25</v>
       </c>
@@ -36470,7 +36470,7 @@
       <c r="CN417" s="13"/>
       <c r="CO417" s="13"/>
     </row>
-    <row r="418" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H418" s="12" t="s">
         <v>28</v>
       </c>
@@ -36564,7 +36564,7 @@
       <c r="CN418" s="13"/>
       <c r="CO418" s="13"/>
     </row>
-    <row r="419" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A419" s="9">
         <f>SUBTOTAL(3,$E$2:E419)</f>
         <v>72</v>
@@ -36675,7 +36675,7 @@
       <c r="CN419" s="13"/>
       <c r="CO419" s="13"/>
     </row>
-    <row r="420" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:93" x14ac:dyDescent="0.25">
       <c r="E420" s="12"/>
       <c r="H420" s="12" t="s">
         <v>22</v>
@@ -36770,7 +36770,7 @@
       <c r="CN420" s="13"/>
       <c r="CO420" s="13"/>
     </row>
-    <row r="421" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:93" x14ac:dyDescent="0.25">
       <c r="E421" s="12"/>
       <c r="H421" s="12" t="s">
         <v>23</v>
@@ -36865,7 +36865,7 @@
       <c r="CN421" s="13"/>
       <c r="CO421" s="13"/>
     </row>
-    <row r="422" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="E422" s="12"/>
       <c r="H422" s="12" t="s">
         <v>25</v>
@@ -36960,7 +36960,7 @@
       <c r="CN422" s="13"/>
       <c r="CO422" s="13"/>
     </row>
-    <row r="423" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A423" s="9">
         <f>SUBTOTAL(3,$E$2:E423)</f>
         <v>73</v>
@@ -37071,7 +37071,7 @@
       <c r="CN423" s="13"/>
       <c r="CO423" s="13"/>
     </row>
-    <row r="424" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H424" s="12" t="s">
         <v>22</v>
       </c>
@@ -37165,7 +37165,7 @@
       <c r="CN424" s="13"/>
       <c r="CO424" s="13"/>
     </row>
-    <row r="425" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H425" s="12" t="s">
         <v>23</v>
       </c>
@@ -37259,7 +37259,7 @@
       <c r="CN425" s="13"/>
       <c r="CO425" s="13"/>
     </row>
-    <row r="426" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H426" s="12" t="s">
         <v>25</v>
       </c>
@@ -37353,7 +37353,7 @@
       <c r="CN426" s="13"/>
       <c r="CO426" s="13"/>
     </row>
-    <row r="427" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H427" s="12" t="s">
         <v>28</v>
       </c>
@@ -37447,7 +37447,7 @@
       <c r="CN427" s="13"/>
       <c r="CO427" s="13"/>
     </row>
-    <row r="428" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H428" s="12" t="s">
         <v>30</v>
       </c>
@@ -37541,7 +37541,7 @@
       <c r="CN428" s="13"/>
       <c r="CO428" s="13"/>
     </row>
-    <row r="429" spans="1:93" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:93" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E429" s="18"/>
       <c r="H429" s="12" t="s">
         <v>32</v>
@@ -37636,7 +37636,7 @@
       <c r="CN429" s="13"/>
       <c r="CO429" s="13"/>
     </row>
-    <row r="430" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A430" s="9">
         <f>SUBTOTAL(3,$E$2:E430)</f>
         <v>74</v>
@@ -37747,7 +37747,7 @@
       <c r="CN430" s="13"/>
       <c r="CO430" s="13"/>
     </row>
-    <row r="431" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H431" s="12" t="s">
         <v>22</v>
       </c>
@@ -37841,7 +37841,7 @@
       <c r="CN431" s="13"/>
       <c r="CO431" s="13"/>
     </row>
-    <row r="432" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H432" s="12" t="s">
         <v>23</v>
       </c>
@@ -37935,7 +37935,7 @@
       <c r="CN432" s="13"/>
       <c r="CO432" s="13"/>
     </row>
-    <row r="433" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H433" s="12" t="s">
         <v>25</v>
       </c>
@@ -38029,7 +38029,7 @@
       <c r="CN433" s="13"/>
       <c r="CO433" s="13"/>
     </row>
-    <row r="434" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A434" s="9">
         <f>SUBTOTAL(3,$E$2:E434)</f>
         <v>75</v>
@@ -38140,7 +38140,7 @@
       <c r="CN434" s="13"/>
       <c r="CO434" s="13"/>
     </row>
-    <row r="435" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H435" s="12" t="s">
         <v>22</v>
       </c>
@@ -38234,7 +38234,7 @@
       <c r="CN435" s="13"/>
       <c r="CO435" s="13"/>
     </row>
-    <row r="436" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H436" s="12" t="s">
         <v>23</v>
       </c>
@@ -38328,7 +38328,7 @@
       <c r="CN436" s="13"/>
       <c r="CO436" s="13"/>
     </row>
-    <row r="437" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H437" s="12" t="s">
         <v>25</v>
       </c>
@@ -38422,7 +38422,7 @@
       <c r="CN437" s="13"/>
       <c r="CO437" s="13"/>
     </row>
-    <row r="438" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H438" s="12" t="s">
         <v>28</v>
       </c>
@@ -38516,7 +38516,7 @@
       <c r="CN438" s="13"/>
       <c r="CO438" s="13"/>
     </row>
-    <row r="439" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A439" s="9">
         <f>SUBTOTAL(3,$E$2:E439)</f>
         <v>76</v>
@@ -38627,7 +38627,7 @@
       <c r="CN439" s="13"/>
       <c r="CO439" s="13"/>
     </row>
-    <row r="440" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H440" s="12" t="s">
         <v>22</v>
       </c>
@@ -38721,7 +38721,7 @@
       <c r="CN440" s="13"/>
       <c r="CO440" s="13"/>
     </row>
-    <row r="441" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H441" s="12" t="s">
         <v>23</v>
       </c>
@@ -38815,7 +38815,7 @@
       <c r="CN441" s="13"/>
       <c r="CO441" s="13"/>
     </row>
-    <row r="442" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H442" s="12" t="s">
         <v>25</v>
       </c>
@@ -38909,7 +38909,7 @@
       <c r="CN442" s="13"/>
       <c r="CO442" s="13"/>
     </row>
-    <row r="443" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A443" s="24"/>
       <c r="B443" s="24"/>
       <c r="C443" s="24"/>
@@ -39010,7 +39010,7 @@
       <c r="CN443" s="13"/>
       <c r="CO443" s="13"/>
     </row>
-    <row r="444" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A444" s="9">
         <f>SUBTOTAL(3,$E$2:E444)</f>
         <v>77</v>
@@ -39121,7 +39121,7 @@
       <c r="CN444" s="13"/>
       <c r="CO444" s="13"/>
     </row>
-    <row r="445" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:93" x14ac:dyDescent="0.25">
       <c r="E445" s="12"/>
       <c r="H445" s="12" t="s">
         <v>22</v>
@@ -39216,7 +39216,7 @@
       <c r="CN445" s="13"/>
       <c r="CO445" s="13"/>
     </row>
-    <row r="446" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:93" x14ac:dyDescent="0.25">
       <c r="E446" s="12"/>
       <c r="H446" s="12" t="s">
         <v>23</v>
@@ -39311,7 +39311,7 @@
       <c r="CN446" s="13"/>
       <c r="CO446" s="13"/>
     </row>
-    <row r="447" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="E447" s="12"/>
       <c r="H447" s="12" t="s">
         <v>25</v>
@@ -39406,7 +39406,7 @@
       <c r="CN447" s="13"/>
       <c r="CO447" s="13"/>
     </row>
-    <row r="448" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A448" s="9">
         <f>SUBTOTAL(3,$E$2:E448)</f>
         <v>78</v>
@@ -39517,7 +39517,7 @@
       <c r="CN448" s="13"/>
       <c r="CO448" s="13"/>
     </row>
-    <row r="449" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:93" x14ac:dyDescent="0.25">
       <c r="E449" s="12"/>
       <c r="H449" s="12" t="s">
         <v>22</v>
@@ -39612,7 +39612,7 @@
       <c r="CN449" s="13"/>
       <c r="CO449" s="13"/>
     </row>
-    <row r="450" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:93" x14ac:dyDescent="0.25">
       <c r="E450" s="12"/>
       <c r="H450" s="12" t="s">
         <v>23</v>
@@ -39707,7 +39707,7 @@
       <c r="CN450" s="13"/>
       <c r="CO450" s="13"/>
     </row>
-    <row r="451" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="E451" s="12"/>
       <c r="H451" s="12" t="s">
         <v>25</v>
@@ -39802,7 +39802,7 @@
       <c r="CN451" s="13"/>
       <c r="CO451" s="13"/>
     </row>
-    <row r="452" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A452" s="9">
         <f>SUBTOTAL(3,$E$2:E452)</f>
         <v>79</v>
@@ -39913,7 +39913,7 @@
       <c r="CN452" s="13"/>
       <c r="CO452" s="13"/>
     </row>
-    <row r="453" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H453" s="12" t="s">
         <v>22</v>
       </c>
@@ -40007,7 +40007,7 @@
       <c r="CN453" s="13"/>
       <c r="CO453" s="13"/>
     </row>
-    <row r="454" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A454" s="9"/>
       <c r="C454" s="10"/>
       <c r="D454" s="11"/>
@@ -40104,7 +40104,7 @@
       <c r="CN454" s="13"/>
       <c r="CO454" s="13"/>
     </row>
-    <row r="455" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H455" s="12" t="s">
         <v>25</v>
       </c>
@@ -40198,7 +40198,7 @@
       <c r="CN455" s="13"/>
       <c r="CO455" s="13"/>
     </row>
-    <row r="456" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A456" s="9">
         <f>SUBTOTAL(3,$E$2:E456)</f>
         <v>80</v>
@@ -40309,7 +40309,7 @@
       <c r="CN456" s="13"/>
       <c r="CO456" s="13"/>
     </row>
-    <row r="457" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H457" s="12" t="s">
         <v>22</v>
       </c>
@@ -40403,7 +40403,7 @@
       <c r="CN457" s="13"/>
       <c r="CO457" s="13"/>
     </row>
-    <row r="458" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H458" s="12" t="s">
         <v>23</v>
       </c>
@@ -40497,7 +40497,7 @@
       <c r="CN458" s="13"/>
       <c r="CO458" s="13"/>
     </row>
-    <row r="459" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="E459" s="12"/>
       <c r="H459" s="12" t="s">
         <v>25</v>
@@ -40592,7 +40592,7 @@
       <c r="CN459" s="13"/>
       <c r="CO459" s="13"/>
     </row>
-    <row r="460" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A460" s="9">
         <f>SUBTOTAL(3,$E$2:E460)</f>
         <v>81</v>
@@ -40703,7 +40703,7 @@
       <c r="CN460" s="13"/>
       <c r="CO460" s="13"/>
     </row>
-    <row r="461" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H461" s="12" t="s">
         <v>22</v>
       </c>
@@ -40797,7 +40797,7 @@
       <c r="CN461" s="13"/>
       <c r="CO461" s="13"/>
     </row>
-    <row r="462" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H462" s="12" t="s">
         <v>23</v>
       </c>
@@ -40891,7 +40891,7 @@
       <c r="CN462" s="13"/>
       <c r="CO462" s="13"/>
     </row>
-    <row r="463" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="E463" s="12"/>
       <c r="H463" s="12" t="s">
         <v>25</v>
@@ -40986,7 +40986,7 @@
       <c r="CN463" s="13"/>
       <c r="CO463" s="13"/>
     </row>
-    <row r="464" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A464" s="9">
         <f>SUBTOTAL(3,$E$2:E464)</f>
         <v>82</v>
@@ -41097,7 +41097,7 @@
       <c r="CN464" s="13"/>
       <c r="CO464" s="13"/>
     </row>
-    <row r="465" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H465" s="12" t="s">
         <v>22</v>
       </c>
@@ -41191,7 +41191,7 @@
       <c r="CN465" s="13"/>
       <c r="CO465" s="13"/>
     </row>
-    <row r="466" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H466" s="12" t="s">
         <v>23</v>
       </c>
@@ -41285,7 +41285,7 @@
       <c r="CN466" s="13"/>
       <c r="CO466" s="13"/>
     </row>
-    <row r="467" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H467" s="12" t="s">
         <v>25</v>
       </c>
@@ -41379,7 +41379,7 @@
       <c r="CN467" s="13"/>
       <c r="CO467" s="13"/>
     </row>
-    <row r="468" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A468" s="9">
         <f>SUBTOTAL(3,$E$2:E468)</f>
         <v>83</v>
@@ -41490,7 +41490,7 @@
       <c r="CN468" s="13"/>
       <c r="CO468" s="13"/>
     </row>
-    <row r="469" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H469" s="12" t="s">
         <v>22</v>
       </c>
@@ -41584,7 +41584,7 @@
       <c r="CN469" s="13"/>
       <c r="CO469" s="13"/>
     </row>
-    <row r="470" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H470" s="12" t="s">
         <v>23</v>
       </c>
@@ -41678,7 +41678,7 @@
       <c r="CN470" s="13"/>
       <c r="CO470" s="13"/>
     </row>
-    <row r="471" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:93" x14ac:dyDescent="0.25">
       <c r="E471" s="12"/>
       <c r="H471" s="12" t="s">
         <v>25</v>
@@ -41773,7 +41773,7 @@
       <c r="CN471" s="13"/>
       <c r="CO471" s="13"/>
     </row>
-    <row r="472" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A472" s="9">
         <f>SUBTOTAL(3,$E$2:E472)</f>
         <v>84</v>
@@ -41884,7 +41884,7 @@
       <c r="CN472" s="13"/>
       <c r="CO472" s="13"/>
     </row>
-    <row r="473" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H473" s="12" t="s">
         <v>22</v>
       </c>
@@ -41978,7 +41978,7 @@
       <c r="CN473" s="13"/>
       <c r="CO473" s="13"/>
     </row>
-    <row r="474" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H474" s="12" t="s">
         <v>23</v>
       </c>
@@ -42072,7 +42072,7 @@
       <c r="CN474" s="13"/>
       <c r="CO474" s="13"/>
     </row>
-    <row r="475" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:93" x14ac:dyDescent="0.25">
       <c r="E475" s="12"/>
       <c r="H475" s="12" t="s">
         <v>25</v>
@@ -42167,7 +42167,7 @@
       <c r="CN475" s="13"/>
       <c r="CO475" s="13"/>
     </row>
-    <row r="476" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A476" s="9">
         <f>SUBTOTAL(3,$E$2:E476)</f>
         <v>85</v>
@@ -42278,7 +42278,7 @@
       <c r="CN476" s="13"/>
       <c r="CO476" s="13"/>
     </row>
-    <row r="477" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H477" s="12" t="s">
         <v>22</v>
       </c>
@@ -42372,7 +42372,7 @@
       <c r="CN477" s="13"/>
       <c r="CO477" s="13"/>
     </row>
-    <row r="478" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H478" s="12" t="s">
         <v>23</v>
       </c>
@@ -42466,7 +42466,7 @@
       <c r="CN478" s="13"/>
       <c r="CO478" s="13"/>
     </row>
-    <row r="479" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H479" s="12" t="s">
         <v>25</v>
       </c>
@@ -42560,7 +42560,7 @@
       <c r="CN479" s="13"/>
       <c r="CO479" s="13"/>
     </row>
-    <row r="480" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H480" s="12" t="s">
         <v>28</v>
       </c>
@@ -42654,7 +42654,7 @@
       <c r="CN480" s="13"/>
       <c r="CO480" s="13"/>
     </row>
-    <row r="481" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H481" s="12" t="s">
         <v>30</v>
       </c>
@@ -42748,7 +42748,7 @@
       <c r="CN481" s="13"/>
       <c r="CO481" s="13"/>
     </row>
-    <row r="482" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A482" s="9">
         <f>SUBTOTAL(3,$E$2:E482)</f>
         <v>86</v>
@@ -42859,7 +42859,7 @@
       <c r="CN482" s="13"/>
       <c r="CO482" s="13"/>
     </row>
-    <row r="483" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H483" s="12" t="s">
         <v>22</v>
       </c>
@@ -42953,7 +42953,7 @@
       <c r="CN483" s="13"/>
       <c r="CO483" s="13"/>
     </row>
-    <row r="484" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H484" s="12" t="s">
         <v>23</v>
       </c>
@@ -43047,7 +43047,7 @@
       <c r="CN484" s="13"/>
       <c r="CO484" s="13"/>
     </row>
-    <row r="485" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H485" s="12" t="s">
         <v>25</v>
       </c>
@@ -43141,7 +43141,7 @@
       <c r="CN485" s="13"/>
       <c r="CO485" s="13"/>
     </row>
-    <row r="486" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H486" s="12" t="s">
         <v>28</v>
       </c>
@@ -43235,7 +43235,7 @@
       <c r="CN486" s="13"/>
       <c r="CO486" s="13"/>
     </row>
-    <row r="487" spans="1:93" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:93" ht="27.6" x14ac:dyDescent="0.25">
       <c r="H487" s="12" t="s">
         <v>30</v>
       </c>
@@ -43329,7 +43329,7 @@
       <c r="CN487" s="13"/>
       <c r="CO487" s="13"/>
     </row>
-    <row r="488" spans="1:93" ht="57" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:93" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A488" s="9">
         <f>SUBTOTAL(3,$E$2:E488)</f>
         <v>87</v>
@@ -43440,7 +43440,7 @@
       <c r="CN488" s="13"/>
       <c r="CO488" s="13"/>
     </row>
-    <row r="489" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H489" s="12" t="s">
         <v>22</v>
       </c>
@@ -43534,7 +43534,7 @@
       <c r="CN489" s="13"/>
       <c r="CO489" s="13"/>
     </row>
-    <row r="490" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H490" s="12" t="s">
         <v>23</v>
       </c>
@@ -43628,7 +43628,7 @@
       <c r="CN490" s="13"/>
       <c r="CO490" s="13"/>
     </row>
-    <row r="491" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:93" x14ac:dyDescent="0.25">
       <c r="H491" s="12" t="s">
         <v>25</v>
       </c>

</xml_diff>